<commit_message>
added birth outcome tabs to spreadsheet
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -9,7 +9,10 @@
     <sheet state="visible" name="RRWasting" sheetId="4" r:id="rId6"/>
     <sheet state="visible" name="RRBreastFeeding" sheetId="5" r:id="rId7"/>
     <sheet state="visible" name="distributions" sheetId="6" r:id="rId8"/>
-    <sheet state="visible" name="birth circumstance" sheetId="7" r:id="rId9"/>
+    <sheet state="visible" name="birth distribution" sheetId="7" r:id="rId9"/>
+    <sheet state="visible" name="time between births" sheetId="8" r:id="rId10"/>
+    <sheet state="visible" name="RR birth by type" sheetId="9" r:id="rId11"/>
+    <sheet state="visible" name="RR birth by time" sheetId="10" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="54">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -169,6 +172,48 @@
   </si>
   <si>
     <t>Breast Feeding</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>&lt;18 years</t>
+  </si>
+  <si>
+    <t>18-34 years</t>
+  </si>
+  <si>
+    <t>35-49 years</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>second or third</t>
+  </si>
+  <si>
+    <t>greater than third</t>
+  </si>
+  <si>
+    <t>&lt;18 months</t>
+  </si>
+  <si>
+    <t>18-23 months</t>
+  </si>
+  <si>
+    <t>&lt;24 months</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>pretermSGA</t>
+  </si>
+  <si>
+    <t>pretermAGA</t>
+  </si>
+  <si>
+    <t>termSGA</t>
   </si>
 </sst>
 </file>
@@ -246,6 +291,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
@@ -270,6 +319,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/worksheetdrawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
@@ -314,6 +371,86 @@
   </sheetData>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.03</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.77</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.49</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.41</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.18</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2499,7 +2636,271 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.0543</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.1711</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3.0E-4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.009</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.3607</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0085</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.2908</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.1048</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>0.2258</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.0705</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.134</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.5698</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.14</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.73</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished adding birth outcomes to spreadsheet and function which reads from it
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -13,6 +13,7 @@
     <sheet state="visible" name="time between births" sheetId="8" r:id="rId10"/>
     <sheet state="visible" name="RR birth by type" sheetId="9" r:id="rId11"/>
     <sheet state="visible" name="RR birth by time" sheetId="10" r:id="rId12"/>
+    <sheet state="visible" name="OR stunting progression" sheetId="11" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="54">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -295,6 +296,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
@@ -454,6 +459,46 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>12.4</v>
+      </c>
+      <c r="B2" s="3">
+        <v>21.4</v>
+      </c>
+      <c r="C2" s="3">
+        <v>30.3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>46.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>

</xml_diff>

<commit_message>
fixed spelling consistency of breastfeeding
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -7,7 +7,7 @@
     <sheet state="visible" name="mortality" sheetId="2" r:id="rId4"/>
     <sheet state="visible" name="RRStunting" sheetId="3" r:id="rId5"/>
     <sheet state="visible" name="RRWasting" sheetId="4" r:id="rId6"/>
-    <sheet state="visible" name="RRBreastFeeding" sheetId="5" r:id="rId7"/>
+    <sheet state="visible" name="RRBreastfeeding" sheetId="5" r:id="rId7"/>
     <sheet state="visible" name="distributions" sheetId="6" r:id="rId8"/>
     <sheet state="visible" name="birth distribution" sheetId="7" r:id="rId9"/>
     <sheet state="visible" name="time between births" sheetId="8" r:id="rId10"/>
@@ -145,7 +145,7 @@
     <t>Casue</t>
   </si>
   <si>
-    <t>Breast Feeding Status</t>
+    <t>Breastfeeding Status</t>
   </si>
   <si>
     <t>exclusive</t>
@@ -172,7 +172,7 @@
     <t>Wasting</t>
   </si>
   <si>
-    <t>Breast Feeding</t>
+    <t>Breastfeeding</t>
   </si>
   <si>
     <t>Type</t>

</xml_diff>

<commit_message>
added birthOutcomeDist to read from spreadsheet and fixed some minor bugs
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -11,9 +11,10 @@
     <sheet state="visible" name="distributions" sheetId="6" r:id="rId8"/>
     <sheet state="visible" name="birth distribution" sheetId="7" r:id="rId9"/>
     <sheet state="visible" name="time between births" sheetId="8" r:id="rId10"/>
-    <sheet state="visible" name="RR birth by type" sheetId="9" r:id="rId11"/>
-    <sheet state="visible" name="RR birth by time" sheetId="10" r:id="rId12"/>
-    <sheet state="visible" name="OR stunting progression" sheetId="11" r:id="rId13"/>
+    <sheet state="visible" name="birth outcome distribution" sheetId="9" r:id="rId11"/>
+    <sheet state="visible" name="RR birth by type" sheetId="10" r:id="rId12"/>
+    <sheet state="visible" name="RR birth by time" sheetId="11" r:id="rId13"/>
+    <sheet state="visible" name="OR stunting progression" sheetId="12" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="54">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -205,16 +206,16 @@
     <t>&lt;24 months</t>
   </si>
   <si>
+    <t>pretermSGA</t>
+  </si>
+  <si>
+    <t>pretermAGA</t>
+  </si>
+  <si>
+    <t>termSGA</t>
+  </si>
+  <si>
     <t>Outcome</t>
-  </si>
-  <si>
-    <t>pretermSGA</t>
-  </si>
-  <si>
-    <t>pretermAGA</t>
-  </si>
-  <si>
-    <t>termSGA</t>
   </si>
 </sst>
 </file>
@@ -300,6 +301,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
@@ -388,69 +393,155 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.14</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.73</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>3.03</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1.77</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.49</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.1</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.41</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.18</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="B8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -460,6 +551,86 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.03</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.77</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.49</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.41</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.18</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2796,153 +2967,21 @@
         <v>50</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>44</v>
+      <c r="A2" s="3">
+        <v>0.0198</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.1032</v>
       </c>
       <c r="C2" s="3">
-        <v>3.14</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1.73</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1.75</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1.75</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1.52</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1.52</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.0</v>
+        <v>0.7419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the way I fixed breastfeeding underlying mortality bug.  Added new spreadsheet where 21-59 month old have 100% in 'none'
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="53">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>Wasting Status</t>
-  </si>
-  <si>
-    <t>Casue</t>
   </si>
   <si>
     <t>Breastfeeding Status</t>
@@ -393,27 +390,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="3">
         <v>3.14</v>
@@ -428,7 +425,7 @@
     <row r="3">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3">
         <v>1.6</v>
@@ -443,7 +440,7 @@
     <row r="4">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3">
         <v>1.6</v>
@@ -457,10 +454,10 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="3">
         <v>1.75</v>
@@ -474,7 +471,7 @@
     </row>
     <row r="6">
       <c r="B6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="3">
         <v>1.4</v>
@@ -488,7 +485,7 @@
     </row>
     <row r="7">
       <c r="B7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="3">
         <v>1.4</v>
@@ -502,10 +499,10 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3">
         <v>1.52</v>
@@ -519,7 +516,7 @@
     </row>
     <row r="9">
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="3">
         <v>1.2</v>
@@ -533,7 +530,7 @@
     </row>
     <row r="10">
       <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="3">
         <v>1.2</v>
@@ -559,24 +556,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3">
         <v>1.0</v>
@@ -593,7 +590,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="3">
         <v>1.0</v>
@@ -610,7 +607,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="3">
         <v>1.0</v>
@@ -1954,10 +1951,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1980,7 +1977,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>1.0</v>
@@ -2000,7 +1997,7 @@
     </row>
     <row r="3">
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>2.28</v>
@@ -2020,7 +2017,7 @@
     </row>
     <row r="4">
       <c r="B4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>4.62</v>
@@ -2040,7 +2037,7 @@
     </row>
     <row r="5">
       <c r="B5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5">
         <v>10.53</v>
@@ -2063,7 +2060,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>1.0</v>
@@ -2083,7 +2080,7 @@
     </row>
     <row r="7">
       <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>2.28</v>
@@ -2103,7 +2100,7 @@
     </row>
     <row r="8">
       <c r="B8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>4.62</v>
@@ -2123,7 +2120,7 @@
     </row>
     <row r="9">
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>10.53</v>
@@ -2146,7 +2143,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>1.0</v>
@@ -2166,7 +2163,7 @@
     </row>
     <row r="11">
       <c r="B11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11">
         <v>2.28</v>
@@ -2186,7 +2183,7 @@
     </row>
     <row r="12">
       <c r="B12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>4.62</v>
@@ -2206,7 +2203,7 @@
     </row>
     <row r="13">
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13">
         <v>10.53</v>
@@ -2229,7 +2226,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>1.0</v>
@@ -2249,7 +2246,7 @@
     </row>
     <row r="15">
       <c r="B15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15">
         <v>2.28</v>
@@ -2269,7 +2266,7 @@
     </row>
     <row r="16">
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16">
         <v>4.62</v>
@@ -2289,7 +2286,7 @@
     </row>
     <row r="17">
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <v>10.53</v>
@@ -2312,7 +2309,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="3">
         <v>1.0</v>
@@ -2332,7 +2329,7 @@
     </row>
     <row r="19">
       <c r="B19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="3">
         <v>1.0</v>
@@ -2352,7 +2349,7 @@
     </row>
     <row r="20">
       <c r="B20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3">
         <v>1.0</v>
@@ -2372,7 +2369,7 @@
     </row>
     <row r="21">
       <c r="B21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3">
         <v>1.0</v>
@@ -2395,7 +2392,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="3">
         <v>1.0</v>
@@ -2415,7 +2412,7 @@
     </row>
     <row r="23">
       <c r="B23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="3">
         <v>1.0</v>
@@ -2435,7 +2432,7 @@
     </row>
     <row r="24">
       <c r="B24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="3">
         <v>1.0</v>
@@ -2455,7 +2452,7 @@
     </row>
     <row r="25">
       <c r="B25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="3">
         <v>1.0</v>
@@ -2478,7 +2475,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="3">
         <v>1.0</v>
@@ -2498,7 +2495,7 @@
     </row>
     <row r="27">
       <c r="B27" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" s="3">
         <v>1.0</v>
@@ -2518,7 +2515,7 @@
     </row>
     <row r="28">
       <c r="B28" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="3">
         <v>1.0</v>
@@ -2538,7 +2535,7 @@
     </row>
     <row r="29">
       <c r="B29" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="3">
         <v>1.0</v>
@@ -2570,10 +2567,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -2593,7 +2590,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>24</v>
@@ -2676,7 +2673,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>24</v>
@@ -2759,10 +2756,10 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="6">
         <v>52.781</v>
@@ -2782,7 +2779,7 @@
     </row>
     <row r="11">
       <c r="B11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="6">
         <v>30.485</v>
@@ -2802,7 +2799,7 @@
     </row>
     <row r="12">
       <c r="B12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="6">
         <v>15.035</v>
@@ -2822,7 +2819,7 @@
     </row>
     <row r="13">
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1">
         <v>1.699</v>
@@ -2837,7 +2834,7 @@
         <v>28.202</v>
       </c>
       <c r="G13" s="3">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
     </row>
   </sheetData>
@@ -2855,22 +2852,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3">
         <v>0.0543</v>
@@ -2884,7 +2881,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3">
         <v>0.009</v>
@@ -2898,7 +2895,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3">
         <v>0.0</v>
@@ -2924,16 +2921,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2">
@@ -2964,13 +2961,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
added OR birth outcome stunting to spreadsheet
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -15,6 +15,7 @@
     <sheet state="visible" name="RR birth by type" sheetId="10" r:id="rId12"/>
     <sheet state="visible" name="RR birth by time" sheetId="11" r:id="rId13"/>
     <sheet state="visible" name="OR stunting progression" sheetId="12" r:id="rId14"/>
+    <sheet state="visible" name="OR birth outcome stunting" sheetId="13" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="57">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -213,6 +214,18 @@
   </si>
   <si>
     <t>Outcome</t>
+  </si>
+  <si>
+    <t>Term AGA</t>
+  </si>
+  <si>
+    <t>Term SGA</t>
+  </si>
+  <si>
+    <t>Pre-term AGA</t>
+  </si>
+  <si>
+    <t>Pre-term SGA</t>
   </si>
 </sst>
 </file>
@@ -254,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -278,6 +291,9 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -299,6 +315,10 @@
 </file>
 
 <file path=xl/drawings/worksheetdrawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/worksheetdrawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -667,6 +687,46 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.82</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.94</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.98</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>

</xml_diff>

<commit_message>
fix strings referring to birth outcomes; rearrange order of sheets
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -5,16 +5,16 @@
   <sheets>
     <sheet state="visible" name="total mortality" sheetId="1" r:id="rId3"/>
     <sheet state="visible" name="mortality" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="RRStunting" sheetId="3" r:id="rId5"/>
-    <sheet state="visible" name="RRWasting" sheetId="4" r:id="rId6"/>
-    <sheet state="visible" name="RRBreastfeeding" sheetId="5" r:id="rId7"/>
-    <sheet state="visible" name="distributions" sheetId="6" r:id="rId8"/>
-    <sheet state="visible" name="birth distribution" sheetId="7" r:id="rId9"/>
-    <sheet state="visible" name="time between births" sheetId="8" r:id="rId10"/>
-    <sheet state="visible" name="birth outcome distribution" sheetId="9" r:id="rId11"/>
-    <sheet state="visible" name="RR birth by type" sheetId="10" r:id="rId12"/>
-    <sheet state="visible" name="RR birth by time" sheetId="11" r:id="rId13"/>
-    <sheet state="visible" name="OR stunting progression" sheetId="12" r:id="rId14"/>
+    <sheet state="visible" name="distributions" sheetId="3" r:id="rId5"/>
+    <sheet state="visible" name="RRStunting" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="RRWasting" sheetId="5" r:id="rId7"/>
+    <sheet state="visible" name="RRBreastfeeding" sheetId="6" r:id="rId8"/>
+    <sheet state="visible" name="OR stunting progression" sheetId="7" r:id="rId9"/>
+    <sheet state="visible" name="birth distribution" sheetId="8" r:id="rId10"/>
+    <sheet state="visible" name="time between births" sheetId="9" r:id="rId11"/>
+    <sheet state="visible" name="birth outcome distribution" sheetId="10" r:id="rId12"/>
+    <sheet state="visible" name="RR birth by type" sheetId="11" r:id="rId13"/>
+    <sheet state="visible" name="RR birth by time" sheetId="12" r:id="rId14"/>
     <sheet state="visible" name="OR birth outcome stunting" sheetId="13" r:id="rId15"/>
   </sheets>
   <definedNames/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="54">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -126,54 +126,54 @@
     <t>Other</t>
   </si>
   <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Stunting</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>mild</t>
+  </si>
+  <si>
+    <t>moderate</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>Wasting</t>
+  </si>
+  <si>
+    <t>Breastfeeding</t>
+  </si>
+  <si>
+    <t>exclusive</t>
+  </si>
+  <si>
+    <t>predominant</t>
+  </si>
+  <si>
+    <t>partial</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
     <t>Stunting Status</t>
   </si>
   <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>mild</t>
-  </si>
-  <si>
-    <t>moderate</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
     <t>Wasting Status</t>
   </si>
   <si>
     <t>Breastfeeding Status</t>
   </si>
   <si>
-    <t>exclusive</t>
-  </si>
-  <si>
-    <t>predominant</t>
-  </si>
-  <si>
-    <t>partial</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>Distribution</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Stunting</t>
-  </si>
-  <si>
-    <t>Wasting</t>
-  </si>
-  <si>
-    <t>Breastfeeding</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -204,28 +204,19 @@
     <t>&lt;24 months</t>
   </si>
   <si>
-    <t>pretermSGA</t>
-  </si>
-  <si>
-    <t>pretermAGA</t>
-  </si>
-  <si>
-    <t>termSGA</t>
+    <t>Pre-term SGA</t>
+  </si>
+  <si>
+    <t>Pre-term AGA</t>
+  </si>
+  <si>
+    <t>Term SGA</t>
   </si>
   <si>
     <t>Outcome</t>
   </si>
   <si>
     <t>Term AGA</t>
-  </si>
-  <si>
-    <t>Term SGA</t>
-  </si>
-  <si>
-    <t>Pre-term AGA</t>
-  </si>
-  <si>
-    <t>Pre-term SGA</t>
   </si>
 </sst>
 </file>
@@ -410,156 +401,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>43</v>
+      <c r="A2" s="3">
+        <v>0.0198</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.1032</v>
       </c>
       <c r="C2" s="3">
-        <v>3.14</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1.73</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1.75</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1.75</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1.52</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1.52</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.0</v>
+        <v>0.7419</v>
       </c>
     </row>
   </sheetData>
@@ -579,66 +438,152 @@
         <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="3">
-        <v>1.0</v>
+      <c r="B2" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="C2" s="3">
-        <v>3.03</v>
+        <v>3.14</v>
       </c>
       <c r="D2" s="3">
-        <v>1.77</v>
+        <v>1.73</v>
       </c>
       <c r="E2" s="3">
-        <v>1.0</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.49</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.1</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.41</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.18</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="B8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -655,31 +600,71 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
+      <c r="A1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3">
-        <v>12.4</v>
+      <c r="A2" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B2" s="3">
-        <v>21.4</v>
+        <v>1.0</v>
       </c>
       <c r="C2" s="3">
-        <v>30.3</v>
+        <v>3.03</v>
       </c>
       <c r="D2" s="3">
-        <v>46.2</v>
+        <v>1.77</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.49</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.41</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.18</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -699,13 +684,13 @@
         <v>53</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
@@ -1108,10 +1093,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1130,422 +1115,257 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>14</v>
+      <c r="A2" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D2">
-        <v>1.0</v>
-      </c>
-      <c r="E2">
-        <v>1.0</v>
-      </c>
-      <c r="F2">
-        <v>1.0</v>
-      </c>
-      <c r="G2">
-        <v>1.0</v>
+        <v>26</v>
+      </c>
+      <c r="C2" s="5">
+        <v>72.414</v>
+      </c>
+      <c r="D2" s="5">
+        <v>72.414</v>
+      </c>
+      <c r="E2" s="5">
+        <v>50.928</v>
+      </c>
+      <c r="F2" s="5">
+        <v>30.281</v>
+      </c>
+      <c r="G2" s="5">
+        <v>30.859</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D3">
-        <v>1.67</v>
-      </c>
-      <c r="E3">
-        <v>1.67</v>
-      </c>
-      <c r="F3">
-        <v>1.67</v>
-      </c>
-      <c r="G3">
-        <v>1.67</v>
+        <v>27</v>
+      </c>
+      <c r="C3" s="5">
+        <v>17.035</v>
+      </c>
+      <c r="D3" s="5">
+        <v>17.035</v>
+      </c>
+      <c r="E3" s="5">
+        <v>22.44</v>
+      </c>
+      <c r="F3" s="5">
+        <v>25.639</v>
+      </c>
+      <c r="G3" s="5">
+        <v>31.548</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D4">
-        <v>2.38</v>
-      </c>
-      <c r="E4">
-        <v>2.38</v>
-      </c>
-      <c r="F4">
-        <v>2.38</v>
-      </c>
-      <c r="G4">
-        <v>2.38</v>
+        <v>28</v>
+      </c>
+      <c r="C4" s="5">
+        <v>6.386</v>
+      </c>
+      <c r="D4" s="5">
+        <v>6.386</v>
+      </c>
+      <c r="E4" s="5">
+        <v>15.042</v>
+      </c>
+      <c r="F4" s="5">
+        <v>25.718</v>
+      </c>
+      <c r="G4" s="5">
+        <v>23.329</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D5">
-        <v>6.33</v>
-      </c>
-      <c r="E5">
-        <v>6.33</v>
-      </c>
-      <c r="F5">
-        <v>6.33</v>
-      </c>
-      <c r="G5">
-        <v>6.33</v>
+        <v>29</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4.165</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4.165</v>
+      </c>
+      <c r="E5" s="5">
+        <v>11.59</v>
+      </c>
+      <c r="F5" s="5">
+        <v>18.362</v>
+      </c>
+      <c r="G5" s="5">
+        <v>14.264</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>15</v>
+      <c r="A6" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D6">
-        <v>1.0</v>
-      </c>
-      <c r="E6">
-        <v>1.0</v>
-      </c>
-      <c r="F6">
-        <v>1.0</v>
-      </c>
-      <c r="G6">
-        <v>1.0</v>
+        <v>26</v>
+      </c>
+      <c r="C6" s="5">
+        <v>78.902</v>
+      </c>
+      <c r="D6" s="5">
+        <v>78.902</v>
+      </c>
+      <c r="E6" s="5">
+        <v>71.711</v>
+      </c>
+      <c r="F6" s="5">
+        <v>81.568</v>
+      </c>
+      <c r="G6" s="5">
+        <v>79.006</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D7">
-        <v>1.55</v>
-      </c>
-      <c r="E7">
-        <v>1.55</v>
-      </c>
-      <c r="F7">
-        <v>1.55</v>
-      </c>
-      <c r="G7">
-        <v>1.55</v>
+        <v>27</v>
+      </c>
+      <c r="C7" s="5">
+        <v>11.952</v>
+      </c>
+      <c r="D7" s="5">
+        <v>11.952</v>
+      </c>
+      <c r="E7" s="5">
+        <v>17.456</v>
+      </c>
+      <c r="F7" s="5">
+        <v>13.323</v>
+      </c>
+      <c r="G7" s="5">
+        <v>15.178</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D8">
-        <v>2.18</v>
-      </c>
-      <c r="E8">
-        <v>2.18</v>
-      </c>
-      <c r="F8">
-        <v>2.18</v>
-      </c>
-      <c r="G8">
-        <v>2.18</v>
+        <v>28</v>
+      </c>
+      <c r="C8" s="5">
+        <v>4.441</v>
+      </c>
+      <c r="D8" s="5">
+        <v>4.441</v>
+      </c>
+      <c r="E8" s="5">
+        <v>9.671</v>
+      </c>
+      <c r="F8" s="5">
+        <v>3.591</v>
+      </c>
+      <c r="G8" s="5">
+        <v>4.166</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D9">
-        <v>6.39</v>
-      </c>
-      <c r="E9">
-        <v>6.39</v>
-      </c>
-      <c r="F9">
-        <v>6.39</v>
-      </c>
-      <c r="G9">
-        <v>6.39</v>
+        <v>29</v>
+      </c>
+      <c r="C9" s="5">
+        <v>4.705</v>
+      </c>
+      <c r="D9" s="5">
+        <v>4.705</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1.162</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1.518</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1.65</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>17</v>
+      <c r="A10" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D10">
-        <v>1.0</v>
-      </c>
-      <c r="E10">
-        <v>1.0</v>
-      </c>
-      <c r="F10">
-        <v>1.0</v>
-      </c>
-      <c r="G10">
-        <v>1.0</v>
+        <v>32</v>
+      </c>
+      <c r="C10" s="6">
+        <v>52.781</v>
+      </c>
+      <c r="D10" s="6">
+        <v>29.554</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D11">
-        <v>1.0</v>
-      </c>
-      <c r="E11">
-        <v>1.0</v>
-      </c>
-      <c r="F11">
-        <v>1.0</v>
-      </c>
-      <c r="G11">
-        <v>1.0</v>
+        <v>33</v>
+      </c>
+      <c r="C11" s="6">
+        <v>30.485</v>
+      </c>
+      <c r="D11" s="6">
+        <v>14.36</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.0</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D12">
-        <v>2.79</v>
-      </c>
-      <c r="E12">
-        <v>2.79</v>
-      </c>
-      <c r="F12">
-        <v>2.79</v>
-      </c>
-      <c r="G12">
-        <v>2.79</v>
+        <v>34</v>
+      </c>
+      <c r="C12" s="6">
+        <v>15.035</v>
+      </c>
+      <c r="D12" s="6">
+        <v>55.307</v>
+      </c>
+      <c r="E12" s="6">
+        <v>96.353</v>
+      </c>
+      <c r="F12" s="6">
+        <v>71.798</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D13">
-        <v>6.01</v>
-      </c>
-      <c r="E13">
-        <v>6.01</v>
-      </c>
-      <c r="F13">
-        <v>6.01</v>
-      </c>
-      <c r="G13">
-        <v>6.01</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D14">
-        <v>1.0</v>
-      </c>
-      <c r="E14">
-        <v>1.0</v>
-      </c>
-      <c r="F14">
-        <v>1.0</v>
-      </c>
-      <c r="G14">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D15">
-        <v>1.0</v>
-      </c>
-      <c r="E15">
-        <v>1.0</v>
-      </c>
-      <c r="F15">
-        <v>1.0</v>
-      </c>
-      <c r="G15">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D16">
-        <v>1.0</v>
-      </c>
-      <c r="E16">
-        <v>1.0</v>
-      </c>
-      <c r="F16">
-        <v>1.0</v>
-      </c>
-      <c r="G16">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D17">
-        <v>1.0</v>
-      </c>
-      <c r="E17">
-        <v>1.0</v>
-      </c>
-      <c r="F17">
-        <v>1.0</v>
-      </c>
-      <c r="G17">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D18">
-        <v>1.0</v>
-      </c>
-      <c r="E18">
-        <v>1.0</v>
-      </c>
-      <c r="F18">
-        <v>1.0</v>
-      </c>
-      <c r="G18">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D19">
-        <v>1.0</v>
-      </c>
-      <c r="E19">
-        <v>1.0</v>
-      </c>
-      <c r="F19">
-        <v>1.0</v>
-      </c>
-      <c r="G19">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D20">
-        <v>1.86</v>
-      </c>
-      <c r="E20">
-        <v>1.86</v>
-      </c>
-      <c r="F20">
-        <v>1.86</v>
-      </c>
-      <c r="G20">
-        <v>1.86</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D21">
-        <v>3.01</v>
-      </c>
-      <c r="E21">
-        <v>3.01</v>
-      </c>
-      <c r="F21">
-        <v>3.01</v>
-      </c>
-      <c r="G21">
-        <v>3.01</v>
+        <v>35</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1.699</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.779</v>
+      </c>
+      <c r="E13" s="6">
+        <v>3.647</v>
+      </c>
+      <c r="F13" s="6">
+        <v>28.202</v>
+      </c>
+      <c r="G13" s="3">
+        <v>100.0</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1561,7 +1381,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1584,7 +1404,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3">
         <v>1.0</v>
@@ -1604,62 +1424,62 @@
     </row>
     <row r="3">
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3" s="3">
         <v>1.0</v>
       </c>
       <c r="D3">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
       <c r="E3">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
       <c r="F3">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
       <c r="G3">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3">
         <v>1.0</v>
       </c>
       <c r="D4">
-        <v>3.41</v>
+        <v>2.38</v>
       </c>
       <c r="E4">
-        <v>3.41</v>
+        <v>2.38</v>
       </c>
       <c r="F4">
-        <v>3.41</v>
+        <v>2.38</v>
       </c>
       <c r="G4">
-        <v>3.41</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3">
         <v>1.0</v>
       </c>
       <c r="D5">
-        <v>12.33</v>
+        <v>6.33</v>
       </c>
       <c r="E5">
-        <v>12.33</v>
+        <v>6.33</v>
       </c>
       <c r="F5">
-        <v>12.33</v>
+        <v>6.33</v>
       </c>
       <c r="G5">
-        <v>12.33</v>
+        <v>6.33</v>
       </c>
     </row>
     <row r="6">
@@ -1667,7 +1487,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3">
         <v>1.0</v>
@@ -1687,62 +1507,62 @@
     </row>
     <row r="7">
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3">
         <v>1.0</v>
       </c>
       <c r="D7">
-        <v>1.92</v>
+        <v>1.55</v>
       </c>
       <c r="E7">
-        <v>1.92</v>
+        <v>1.55</v>
       </c>
       <c r="F7">
-        <v>1.92</v>
+        <v>1.55</v>
       </c>
       <c r="G7">
-        <v>1.92</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C8" s="3">
         <v>1.0</v>
       </c>
       <c r="D8">
-        <v>4.66</v>
+        <v>2.18</v>
       </c>
       <c r="E8">
-        <v>4.66</v>
+        <v>2.18</v>
       </c>
       <c r="F8">
-        <v>4.66</v>
+        <v>2.18</v>
       </c>
       <c r="G8">
-        <v>4.66</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3">
         <v>1.0</v>
       </c>
       <c r="D9">
-        <v>9.68</v>
+        <v>6.39</v>
       </c>
       <c r="E9">
-        <v>9.68</v>
+        <v>6.39</v>
       </c>
       <c r="F9">
-        <v>9.68</v>
+        <v>6.39</v>
       </c>
       <c r="G9">
-        <v>9.68</v>
+        <v>6.39</v>
       </c>
     </row>
     <row r="10">
@@ -1750,7 +1570,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3">
         <v>1.0</v>
@@ -1770,7 +1590,7 @@
     </row>
     <row r="11">
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3">
         <v>1.0</v>
@@ -1790,42 +1610,42 @@
     </row>
     <row r="12">
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3">
         <v>1.0</v>
       </c>
       <c r="D12">
-        <v>2.58</v>
+        <v>2.79</v>
       </c>
       <c r="E12">
-        <v>2.58</v>
+        <v>2.79</v>
       </c>
       <c r="F12">
-        <v>2.58</v>
+        <v>2.79</v>
       </c>
       <c r="G12">
-        <v>2.58</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3">
         <v>1.0</v>
       </c>
       <c r="D13">
-        <v>9.63</v>
+        <v>6.01</v>
       </c>
       <c r="E13">
-        <v>9.63</v>
+        <v>6.01</v>
       </c>
       <c r="F13">
-        <v>9.63</v>
+        <v>6.01</v>
       </c>
       <c r="G13">
-        <v>9.63</v>
+        <v>6.01</v>
       </c>
     </row>
     <row r="14">
@@ -1833,7 +1653,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C14" s="3">
         <v>1.0</v>
@@ -1853,7 +1673,7 @@
     </row>
     <row r="15">
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3">
         <v>1.0</v>
@@ -1873,7 +1693,7 @@
     </row>
     <row r="16">
       <c r="B16" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3">
         <v>1.0</v>
@@ -1893,7 +1713,7 @@
     </row>
     <row r="17">
       <c r="B17" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3">
         <v>1.0</v>
@@ -1916,7 +1736,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C18" s="3">
         <v>1.0</v>
@@ -1936,62 +1756,62 @@
     </row>
     <row r="19">
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19" s="3">
         <v>1.0</v>
       </c>
       <c r="D19">
-        <v>1.65</v>
+        <v>1.0</v>
       </c>
       <c r="E19">
-        <v>1.65</v>
+        <v>1.0</v>
       </c>
       <c r="F19">
-        <v>1.65</v>
+        <v>1.0</v>
       </c>
       <c r="G19">
-        <v>1.65</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C20" s="3">
         <v>1.0</v>
       </c>
       <c r="D20">
-        <v>2.73</v>
+        <v>1.86</v>
       </c>
       <c r="E20">
-        <v>2.73</v>
+        <v>1.86</v>
       </c>
       <c r="F20">
-        <v>2.73</v>
+        <v>1.86</v>
       </c>
       <c r="G20">
-        <v>2.73</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C21" s="3">
         <v>1.0</v>
       </c>
       <c r="D21">
-        <v>11.21</v>
+        <v>3.01</v>
       </c>
       <c r="E21">
-        <v>11.21</v>
+        <v>3.01</v>
       </c>
       <c r="F21">
-        <v>11.21</v>
+        <v>3.01</v>
       </c>
       <c r="G21">
-        <v>11.21</v>
+        <v>3.01</v>
       </c>
     </row>
   </sheetData>
@@ -2000,6 +1820,456 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D2">
+        <v>1.0</v>
+      </c>
+      <c r="E2">
+        <v>1.0</v>
+      </c>
+      <c r="F2">
+        <v>1.0</v>
+      </c>
+      <c r="G2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D3">
+        <v>1.6</v>
+      </c>
+      <c r="E3">
+        <v>1.6</v>
+      </c>
+      <c r="F3">
+        <v>1.6</v>
+      </c>
+      <c r="G3">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D4">
+        <v>3.41</v>
+      </c>
+      <c r="E4">
+        <v>3.41</v>
+      </c>
+      <c r="F4">
+        <v>3.41</v>
+      </c>
+      <c r="G4">
+        <v>3.41</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D5">
+        <v>12.33</v>
+      </c>
+      <c r="E5">
+        <v>12.33</v>
+      </c>
+      <c r="F5">
+        <v>12.33</v>
+      </c>
+      <c r="G5">
+        <v>12.33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D6">
+        <v>1.0</v>
+      </c>
+      <c r="E6">
+        <v>1.0</v>
+      </c>
+      <c r="F6">
+        <v>1.0</v>
+      </c>
+      <c r="G6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D7">
+        <v>1.92</v>
+      </c>
+      <c r="E7">
+        <v>1.92</v>
+      </c>
+      <c r="F7">
+        <v>1.92</v>
+      </c>
+      <c r="G7">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D8">
+        <v>4.66</v>
+      </c>
+      <c r="E8">
+        <v>4.66</v>
+      </c>
+      <c r="F8">
+        <v>4.66</v>
+      </c>
+      <c r="G8">
+        <v>4.66</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D9">
+        <v>9.68</v>
+      </c>
+      <c r="E9">
+        <v>9.68</v>
+      </c>
+      <c r="F9">
+        <v>9.68</v>
+      </c>
+      <c r="G9">
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D10">
+        <v>1.0</v>
+      </c>
+      <c r="E10">
+        <v>1.0</v>
+      </c>
+      <c r="F10">
+        <v>1.0</v>
+      </c>
+      <c r="G10">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D11">
+        <v>1.0</v>
+      </c>
+      <c r="E11">
+        <v>1.0</v>
+      </c>
+      <c r="F11">
+        <v>1.0</v>
+      </c>
+      <c r="G11">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D12">
+        <v>2.58</v>
+      </c>
+      <c r="E12">
+        <v>2.58</v>
+      </c>
+      <c r="F12">
+        <v>2.58</v>
+      </c>
+      <c r="G12">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D13">
+        <v>9.63</v>
+      </c>
+      <c r="E13">
+        <v>9.63</v>
+      </c>
+      <c r="F13">
+        <v>9.63</v>
+      </c>
+      <c r="G13">
+        <v>9.63</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D14">
+        <v>1.0</v>
+      </c>
+      <c r="E14">
+        <v>1.0</v>
+      </c>
+      <c r="F14">
+        <v>1.0</v>
+      </c>
+      <c r="G14">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D15">
+        <v>1.0</v>
+      </c>
+      <c r="E15">
+        <v>1.0</v>
+      </c>
+      <c r="F15">
+        <v>1.0</v>
+      </c>
+      <c r="G15">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D16">
+        <v>1.0</v>
+      </c>
+      <c r="E16">
+        <v>1.0</v>
+      </c>
+      <c r="F16">
+        <v>1.0</v>
+      </c>
+      <c r="G16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D17">
+        <v>1.0</v>
+      </c>
+      <c r="E17">
+        <v>1.0</v>
+      </c>
+      <c r="F17">
+        <v>1.0</v>
+      </c>
+      <c r="G17">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D18">
+        <v>1.0</v>
+      </c>
+      <c r="E18">
+        <v>1.0</v>
+      </c>
+      <c r="F18">
+        <v>1.0</v>
+      </c>
+      <c r="G18">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D19">
+        <v>1.65</v>
+      </c>
+      <c r="E19">
+        <v>1.65</v>
+      </c>
+      <c r="F19">
+        <v>1.65</v>
+      </c>
+      <c r="G19">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D20">
+        <v>2.73</v>
+      </c>
+      <c r="E20">
+        <v>2.73</v>
+      </c>
+      <c r="F20">
+        <v>2.73</v>
+      </c>
+      <c r="G20">
+        <v>2.73</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D21">
+        <v>11.21</v>
+      </c>
+      <c r="E21">
+        <v>11.21</v>
+      </c>
+      <c r="F21">
+        <v>11.21</v>
+      </c>
+      <c r="G21">
+        <v>11.21</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2014,7 +2284,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -2037,7 +2307,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>1.0</v>
@@ -2057,7 +2327,7 @@
     </row>
     <row r="3">
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>2.28</v>
@@ -2077,7 +2347,7 @@
     </row>
     <row r="4">
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4">
         <v>4.62</v>
@@ -2097,7 +2367,7 @@
     </row>
     <row r="5">
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5">
         <v>10.53</v>
@@ -2120,7 +2390,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>1.0</v>
@@ -2140,7 +2410,7 @@
     </row>
     <row r="7">
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>2.28</v>
@@ -2160,7 +2430,7 @@
     </row>
     <row r="8">
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>4.62</v>
@@ -2180,7 +2450,7 @@
     </row>
     <row r="9">
       <c r="B9" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>10.53</v>
@@ -2203,7 +2473,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>1.0</v>
@@ -2223,7 +2493,7 @@
     </row>
     <row r="11">
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C11">
         <v>2.28</v>
@@ -2243,7 +2513,7 @@
     </row>
     <row r="12">
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12">
         <v>4.62</v>
@@ -2263,7 +2533,7 @@
     </row>
     <row r="13">
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C13">
         <v>10.53</v>
@@ -2286,7 +2556,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>1.0</v>
@@ -2306,7 +2576,7 @@
     </row>
     <row r="15">
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C15">
         <v>2.28</v>
@@ -2326,7 +2596,7 @@
     </row>
     <row r="16">
       <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>4.62</v>
@@ -2346,7 +2616,7 @@
     </row>
     <row r="17">
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C17">
         <v>10.53</v>
@@ -2369,7 +2639,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C18" s="3">
         <v>1.0</v>
@@ -2389,7 +2659,7 @@
     </row>
     <row r="19">
       <c r="B19" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C19" s="3">
         <v>1.0</v>
@@ -2409,7 +2679,7 @@
     </row>
     <row r="20">
       <c r="B20" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C20" s="3">
         <v>1.0</v>
@@ -2429,7 +2699,7 @@
     </row>
     <row r="21">
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C21" s="3">
         <v>1.0</v>
@@ -2452,7 +2722,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C22" s="3">
         <v>1.0</v>
@@ -2472,7 +2742,7 @@
     </row>
     <row r="23">
       <c r="B23" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C23" s="3">
         <v>1.0</v>
@@ -2492,7 +2762,7 @@
     </row>
     <row r="24">
       <c r="B24" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C24" s="3">
         <v>1.0</v>
@@ -2512,7 +2782,7 @@
     </row>
     <row r="25">
       <c r="B25" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C25" s="3">
         <v>1.0</v>
@@ -2535,7 +2805,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3">
         <v>1.0</v>
@@ -2555,7 +2825,7 @@
     </row>
     <row r="27">
       <c r="B27" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C27" s="3">
         <v>1.0</v>
@@ -2575,7 +2845,7 @@
     </row>
     <row r="28">
       <c r="B28" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C28" s="3">
         <v>1.0</v>
@@ -2595,7 +2865,7 @@
     </row>
     <row r="29">
       <c r="B29" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C29" s="3">
         <v>1.0</v>
@@ -2615,291 +2885,6 @@
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="5">
-        <v>72.414</v>
-      </c>
-      <c r="D2" s="5">
-        <v>72.414</v>
-      </c>
-      <c r="E2" s="5">
-        <v>50.928</v>
-      </c>
-      <c r="F2" s="5">
-        <v>30.281</v>
-      </c>
-      <c r="G2" s="5">
-        <v>30.859</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="5">
-        <v>17.035</v>
-      </c>
-      <c r="D3" s="5">
-        <v>17.035</v>
-      </c>
-      <c r="E3" s="5">
-        <v>22.44</v>
-      </c>
-      <c r="F3" s="5">
-        <v>25.639</v>
-      </c>
-      <c r="G3" s="5">
-        <v>31.548</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="5">
-        <v>6.386</v>
-      </c>
-      <c r="D4" s="5">
-        <v>6.386</v>
-      </c>
-      <c r="E4" s="5">
-        <v>15.042</v>
-      </c>
-      <c r="F4" s="5">
-        <v>25.718</v>
-      </c>
-      <c r="G4" s="5">
-        <v>23.329</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="5">
-        <v>4.165</v>
-      </c>
-      <c r="D5" s="5">
-        <v>4.165</v>
-      </c>
-      <c r="E5" s="5">
-        <v>11.59</v>
-      </c>
-      <c r="F5" s="5">
-        <v>18.362</v>
-      </c>
-      <c r="G5" s="5">
-        <v>14.264</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="5">
-        <v>78.902</v>
-      </c>
-      <c r="D6" s="5">
-        <v>78.902</v>
-      </c>
-      <c r="E6" s="5">
-        <v>71.711</v>
-      </c>
-      <c r="F6" s="5">
-        <v>81.568</v>
-      </c>
-      <c r="G6" s="5">
-        <v>79.006</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="5">
-        <v>11.952</v>
-      </c>
-      <c r="D7" s="5">
-        <v>11.952</v>
-      </c>
-      <c r="E7" s="5">
-        <v>17.456</v>
-      </c>
-      <c r="F7" s="5">
-        <v>13.323</v>
-      </c>
-      <c r="G7" s="5">
-        <v>15.178</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="5">
-        <v>4.441</v>
-      </c>
-      <c r="D8" s="5">
-        <v>4.441</v>
-      </c>
-      <c r="E8" s="5">
-        <v>9.671</v>
-      </c>
-      <c r="F8" s="5">
-        <v>3.591</v>
-      </c>
-      <c r="G8" s="5">
-        <v>4.166</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="5">
-        <v>4.705</v>
-      </c>
-      <c r="D9" s="5">
-        <v>4.705</v>
-      </c>
-      <c r="E9" s="5">
-        <v>1.162</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1.518</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1.65</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="6">
-        <v>52.781</v>
-      </c>
-      <c r="D10" s="6">
-        <v>29.554</v>
-      </c>
-      <c r="E10" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="F10" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="6">
-        <v>30.485</v>
-      </c>
-      <c r="D11" s="6">
-        <v>14.36</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="6">
-        <v>15.035</v>
-      </c>
-      <c r="D12" s="6">
-        <v>55.307</v>
-      </c>
-      <c r="E12" s="6">
-        <v>96.353</v>
-      </c>
-      <c r="F12" s="6">
-        <v>71.798</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1.699</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.779</v>
-      </c>
-      <c r="E13" s="6">
-        <v>3.647</v>
-      </c>
-      <c r="F13" s="6">
-        <v>28.202</v>
-      </c>
-      <c r="G13" s="3">
-        <v>100.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2911,60 +2896,31 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="3"/>
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>43</v>
+      <c r="A2" s="3">
+        <v>12.4</v>
       </c>
       <c r="B2" s="3">
-        <v>0.0543</v>
+        <v>21.4</v>
       </c>
       <c r="C2" s="3">
-        <v>0.1711</v>
+        <v>30.3</v>
       </c>
       <c r="D2" s="3">
-        <v>3.0E-4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.009</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.3607</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.0085</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.2908</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.1048</v>
+        <v>46.2</v>
       </c>
     </row>
   </sheetData>
@@ -2981,30 +2937,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>0.2258</v>
-      </c>
       <c r="B2" s="3">
-        <v>0.0705</v>
+        <v>0.0543</v>
       </c>
       <c r="C2" s="3">
-        <v>0.134</v>
+        <v>0.1711</v>
       </c>
       <c r="D2" s="3">
-        <v>0.5698</v>
+        <v>3.0E-4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.009</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.3607</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0085</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.2908</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.1048</v>
       </c>
     </row>
   </sheetData>
@@ -3021,24 +3006,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3">
-        <v>0.0198</v>
+        <v>0.2258</v>
       </c>
       <c r="B2" s="3">
-        <v>0.1032</v>
+        <v>0.0705</v>
       </c>
       <c r="C2" s="3">
-        <v>0.7419</v>
+        <v>0.134</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.5698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add stunting OR given diarrhoea
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -10,14 +10,15 @@
     <sheet state="visible" name="RRWasting" sheetId="5" r:id="rId7"/>
     <sheet state="visible" name="RRBreastfeeding" sheetId="6" r:id="rId8"/>
     <sheet state="visible" name="OR stunting progression" sheetId="7" r:id="rId9"/>
-    <sheet state="visible" name="Incidence Diarrhoea" sheetId="8" r:id="rId10"/>
+    <sheet state="visible" name="Incidence diarrhoea" sheetId="8" r:id="rId10"/>
     <sheet state="visible" name="RR diarrhoea" sheetId="9" r:id="rId11"/>
-    <sheet state="visible" name="birth distribution" sheetId="10" r:id="rId12"/>
-    <sheet state="visible" name="time between births" sheetId="11" r:id="rId13"/>
-    <sheet state="visible" name="birth outcome distribution" sheetId="12" r:id="rId14"/>
-    <sheet state="visible" name="RR birth by type" sheetId="13" r:id="rId15"/>
-    <sheet state="visible" name="RR birth by time" sheetId="14" r:id="rId16"/>
-    <sheet state="visible" name="OR birth outcome stunting" sheetId="15" r:id="rId17"/>
+    <sheet state="visible" name="OR stunting diarrhoea" sheetId="10" r:id="rId12"/>
+    <sheet state="visible" name="birth distribution" sheetId="11" r:id="rId13"/>
+    <sheet state="visible" name="time between births" sheetId="12" r:id="rId14"/>
+    <sheet state="visible" name="birth outcome distribution" sheetId="13" r:id="rId15"/>
+    <sheet state="visible" name="RR birth by type" sheetId="14" r:id="rId16"/>
+    <sheet state="visible" name="RR birth by time" sheetId="15" r:id="rId17"/>
+    <sheet state="visible" name="OR birth outcome stunting" sheetId="16" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="55">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -330,6 +331,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
@@ -417,60 +422,37 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="3"/>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.0543</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.1711</v>
-      </c>
-      <c r="D2" s="3">
-        <v>3.0E-4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.009</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.3607</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.0085</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.2908</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.1048</v>
+      <c r="A2">
+        <v>1.04</v>
+      </c>
+      <c r="B2">
+        <v>1.04</v>
+      </c>
+      <c r="C2">
+        <v>1.04</v>
+      </c>
+      <c r="D2">
+        <v>1.04</v>
+      </c>
+      <c r="E2">
+        <v>1.04</v>
       </c>
     </row>
   </sheetData>
@@ -487,30 +469,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>0.2258</v>
-      </c>
       <c r="B2" s="3">
-        <v>0.0705</v>
+        <v>0.0543</v>
       </c>
       <c r="C2" s="3">
-        <v>0.134</v>
+        <v>0.1711</v>
       </c>
       <c r="D2" s="3">
-        <v>0.5698</v>
+        <v>3.0E-4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.009</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.3607</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0085</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.2908</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.1048</v>
       </c>
     </row>
   </sheetData>
@@ -527,24 +538,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3">
-        <v>0.0198</v>
+        <v>0.2258</v>
       </c>
       <c r="B2" s="3">
-        <v>0.1032</v>
+        <v>0.0705</v>
       </c>
       <c r="C2" s="3">
-        <v>0.7419</v>
+        <v>0.134</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.5698</v>
       </c>
     </row>
   </sheetData>
@@ -561,156 +578,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>44</v>
+      <c r="A2" s="3">
+        <v>0.0198</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.1032</v>
       </c>
       <c r="C2" s="3">
-        <v>3.14</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1.73</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1.75</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1.75</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1.52</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1.52</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.0</v>
+        <v>0.7419</v>
       </c>
     </row>
   </sheetData>
@@ -730,22 +615,188 @@
         <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.14</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.73</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="B2" s="3">
         <v>1.0</v>
       </c>
@@ -798,7 +849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
add RR death by birth outcome; simplify other test numbers
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -9,16 +9,17 @@
     <sheet state="visible" name="RRStunting" sheetId="4" r:id="rId6"/>
     <sheet state="visible" name="RRWasting" sheetId="5" r:id="rId7"/>
     <sheet state="visible" name="RRBreastfeeding" sheetId="6" r:id="rId8"/>
-    <sheet state="visible" name="OR stunting progression" sheetId="7" r:id="rId9"/>
-    <sheet state="visible" name="Incidence diarrhoea" sheetId="8" r:id="rId10"/>
-    <sheet state="visible" name="RR diarrhoea" sheetId="9" r:id="rId11"/>
-    <sheet state="visible" name="OR stunting diarrhoea" sheetId="10" r:id="rId12"/>
-    <sheet state="visible" name="birth distribution" sheetId="11" r:id="rId13"/>
-    <sheet state="visible" name="time between births" sheetId="12" r:id="rId14"/>
-    <sheet state="visible" name="birth outcome distribution" sheetId="13" r:id="rId15"/>
-    <sheet state="visible" name="RR birth by type" sheetId="14" r:id="rId16"/>
-    <sheet state="visible" name="RR birth by time" sheetId="15" r:id="rId17"/>
-    <sheet state="visible" name="OR birth outcome stunting" sheetId="16" r:id="rId18"/>
+    <sheet state="visible" name="RR Death by Birth Outcome" sheetId="7" r:id="rId9"/>
+    <sheet state="visible" name="OR stunting progression" sheetId="8" r:id="rId10"/>
+    <sheet state="visible" name="Incidence diarrhoea" sheetId="9" r:id="rId11"/>
+    <sheet state="visible" name="RR diarrhoea" sheetId="10" r:id="rId12"/>
+    <sheet state="visible" name="OR stunting diarrhoea" sheetId="11" r:id="rId13"/>
+    <sheet state="visible" name="birth distribution" sheetId="12" r:id="rId14"/>
+    <sheet state="visible" name="time between births" sheetId="13" r:id="rId15"/>
+    <sheet state="visible" name="birth outcome distribution" sheetId="14" r:id="rId16"/>
+    <sheet state="visible" name="RR birth by type" sheetId="15" r:id="rId17"/>
+    <sheet state="visible" name="RR birth by time" sheetId="16" r:id="rId18"/>
+    <sheet state="visible" name="OR birth outcome stunting" sheetId="17" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="56">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -177,6 +178,21 @@
     <t>Breastfeeding Status</t>
   </si>
   <si>
+    <t>Term AGA</t>
+  </si>
+  <si>
+    <t>Term SGA</t>
+  </si>
+  <si>
+    <t>Pre-term AGA</t>
+  </si>
+  <si>
+    <t>Pre-term SGA</t>
+  </si>
+  <si>
+    <t>Neonatal congenital anomalies</t>
+  </si>
+  <si>
     <t>Breastfeeding Category</t>
   </si>
   <si>
@@ -210,19 +226,7 @@
     <t>&lt;24 months</t>
   </si>
   <si>
-    <t>Pre-term SGA</t>
-  </si>
-  <si>
-    <t>Pre-term AGA</t>
-  </si>
-  <si>
-    <t>Term SGA</t>
-  </si>
-  <si>
     <t>Outcome</t>
-  </si>
-  <si>
-    <t>Term AGA</t>
   </si>
 </sst>
 </file>
@@ -267,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -291,6 +295,7 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
@@ -335,6 +340,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
@@ -420,39 +429,108 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="25.86"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>1.04</v>
+      <c r="A2" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B2">
-        <v>1.04</v>
+        <v>1.0</v>
       </c>
       <c r="C2">
-        <v>1.04</v>
+        <v>1.0</v>
       </c>
       <c r="D2">
-        <v>1.04</v>
+        <v>1.0</v>
       </c>
       <c r="E2">
-        <v>1.04</v>
+        <v>1.0</v>
+      </c>
+      <c r="F2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>1.26</v>
+      </c>
+      <c r="C3">
+        <v>1.26</v>
+      </c>
+      <c r="D3">
+        <v>1.0</v>
+      </c>
+      <c r="E3">
+        <v>1.0</v>
+      </c>
+      <c r="F3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>1.68</v>
+      </c>
+      <c r="C4">
+        <v>1.68</v>
+      </c>
+      <c r="D4">
+        <v>1.0</v>
+      </c>
+      <c r="E4">
+        <v>1.0</v>
+      </c>
+      <c r="F4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>2.65</v>
+      </c>
+      <c r="C5">
+        <v>2.65</v>
+      </c>
+      <c r="D5">
+        <v>2.07</v>
+      </c>
+      <c r="E5">
+        <v>2.07</v>
+      </c>
+      <c r="F5">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -468,60 +546,37 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="3"/>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.0543</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.1711</v>
-      </c>
-      <c r="D2" s="3">
-        <v>3.0E-4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.009</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.3607</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.0085</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.2908</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.1048</v>
+      <c r="A2">
+        <v>1.04</v>
+      </c>
+      <c r="B2">
+        <v>1.04</v>
+      </c>
+      <c r="C2">
+        <v>1.04</v>
+      </c>
+      <c r="D2">
+        <v>1.04</v>
+      </c>
+      <c r="E2">
+        <v>1.04</v>
       </c>
     </row>
   </sheetData>
@@ -538,30 +593,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>0.2258</v>
-      </c>
       <c r="B2" s="3">
-        <v>0.0705</v>
+        <v>0.0543</v>
       </c>
       <c r="C2" s="3">
-        <v>0.134</v>
+        <v>0.1711</v>
       </c>
       <c r="D2" s="3">
-        <v>0.5698</v>
+        <v>3.0E-4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.009</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.3607</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0085</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.2908</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.1048</v>
       </c>
     </row>
   </sheetData>
@@ -578,24 +662,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3">
-        <v>0.0198</v>
+        <v>0.2258</v>
       </c>
       <c r="B2" s="3">
-        <v>0.1032</v>
+        <v>0.0705</v>
       </c>
       <c r="C2" s="3">
-        <v>0.7419</v>
+        <v>0.134</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.5698</v>
       </c>
     </row>
   </sheetData>
@@ -612,156 +702,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>44</v>
+      <c r="A2" s="3">
+        <v>0.0198</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.1032</v>
       </c>
       <c r="C2" s="3">
-        <v>3.14</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1.73</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1.75</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1.75</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1.52</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1.52</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.0</v>
+        <v>0.7419</v>
       </c>
     </row>
   </sheetData>
@@ -778,69 +736,155 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.14</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.73</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>3.03</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1.77</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="C3" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.49</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.1</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1.0</v>
-      </c>
       <c r="C4" s="3">
-        <v>1.41</v>
+        <v>1.6</v>
       </c>
       <c r="D4" s="3">
-        <v>1.18</v>
+        <v>1.0</v>
       </c>
       <c r="E4" s="3">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -857,17 +901,97 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>50</v>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.03</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.77</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.49</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.41</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.18</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2">
@@ -3071,34 +3195,283 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="33.86"/>
+    <col customWidth="1" min="2" max="2" width="15.57"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3">
-        <v>12.4</v>
-      </c>
-      <c r="B2" s="3">
-        <v>21.4</v>
-      </c>
-      <c r="C2" s="3">
-        <v>30.3</v>
-      </c>
-      <c r="D2" s="3">
-        <v>46.2</v>
-      </c>
+      <c r="A2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C2">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C3">
+        <v>2.07</v>
+      </c>
+      <c r="D3" s="9">
+        <v>8.02</v>
+      </c>
+      <c r="E3" s="9">
+        <v>11.54</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C4">
+        <v>2.07</v>
+      </c>
+      <c r="D4" s="9">
+        <v>8.02</v>
+      </c>
+      <c r="E4" s="9">
+        <v>11.54</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C5">
+        <v>2.07</v>
+      </c>
+      <c r="D5" s="9">
+        <v>8.02</v>
+      </c>
+      <c r="E5" s="9">
+        <v>11.54</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C6">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="9">
+        <v>999.99</v>
+      </c>
+      <c r="E6" s="9">
+        <v>999.99</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C7">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C8">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C9">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13">
+      <c r="B13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -3114,36 +3487,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="9">
-        <v>0.23981666666666668</v>
-      </c>
-      <c r="B2" s="9">
-        <v>0.23981666666666668</v>
-      </c>
-      <c r="C2" s="9">
-        <v>0.36586416666666666</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0.29612333333333335</v>
-      </c>
-      <c r="E2" s="9">
-        <v>0.18924083333333333</v>
+      <c r="A2" s="3">
+        <v>12.4</v>
+      </c>
+      <c r="B2" s="3">
+        <v>21.4</v>
+      </c>
+      <c r="C2" s="3">
+        <v>30.3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>46.2</v>
       </c>
     </row>
   </sheetData>
@@ -3157,108 +3524,39 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="25.86"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>39</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2">
-        <v>1.0</v>
-      </c>
-      <c r="C2">
-        <v>1.0</v>
-      </c>
-      <c r="D2">
-        <v>1.0</v>
-      </c>
-      <c r="E2">
-        <v>1.0</v>
-      </c>
-      <c r="F2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3">
-        <v>1.26</v>
-      </c>
-      <c r="C3">
-        <v>1.26</v>
-      </c>
-      <c r="D3">
-        <v>1.0</v>
-      </c>
-      <c r="E3">
-        <v>1.0</v>
-      </c>
-      <c r="F3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4">
-        <v>1.68</v>
-      </c>
-      <c r="C4">
-        <v>1.68</v>
-      </c>
-      <c r="D4">
-        <v>1.0</v>
-      </c>
-      <c r="E4">
-        <v>1.0</v>
-      </c>
-      <c r="F4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5">
-        <v>2.65</v>
-      </c>
-      <c r="C5">
-        <v>2.65</v>
-      </c>
-      <c r="D5">
-        <v>2.07</v>
-      </c>
-      <c r="E5">
-        <v>2.07</v>
-      </c>
-      <c r="F5">
-        <v>1.0</v>
+      <c r="A2" s="10">
+        <v>0.23981666666666668</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0.23981666666666668</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.36586416666666666</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0.29612333333333335</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0.18924083333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add OR stunting given Zinc; preliminary intervention coverages
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -14,12 +14,14 @@
     <sheet state="visible" name="Incidence diarrhoea" sheetId="9" r:id="rId11"/>
     <sheet state="visible" name="RR diarrhoea" sheetId="10" r:id="rId12"/>
     <sheet state="visible" name="OR stunting diarrhoea" sheetId="11" r:id="rId13"/>
-    <sheet state="visible" name="birth distribution" sheetId="12" r:id="rId14"/>
-    <sheet state="visible" name="time between births" sheetId="13" r:id="rId15"/>
-    <sheet state="visible" name="birth outcome distribution" sheetId="14" r:id="rId16"/>
-    <sheet state="visible" name="RR birth by type" sheetId="15" r:id="rId17"/>
-    <sheet state="visible" name="RR birth by time" sheetId="16" r:id="rId18"/>
-    <sheet state="visible" name="OR birth outcome stunting" sheetId="17" r:id="rId19"/>
+    <sheet state="visible" name="OR stunting Zinc" sheetId="12" r:id="rId14"/>
+    <sheet state="visible" name="birth distribution" sheetId="13" r:id="rId15"/>
+    <sheet state="visible" name="time between births" sheetId="14" r:id="rId16"/>
+    <sheet state="visible" name="birth outcome distribution" sheetId="15" r:id="rId17"/>
+    <sheet state="visible" name="RR birth by type" sheetId="16" r:id="rId18"/>
+    <sheet state="visible" name="RR birth by time" sheetId="17" r:id="rId19"/>
+    <sheet state="visible" name="OR birth outcome stunting" sheetId="18" r:id="rId20"/>
+    <sheet state="visible" name="Intervention coverages" sheetId="19" r:id="rId21"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="60">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -227,6 +229,18 @@
   </si>
   <si>
     <t>Outcome</t>
+  </si>
+  <si>
+    <t>Intervention</t>
+  </si>
+  <si>
+    <t>pre-2016</t>
+  </si>
+  <si>
+    <t>Zinc supplementation</t>
+  </si>
+  <si>
+    <t>Vitamin A supplementation</t>
   </si>
 </sst>
 </file>
@@ -344,6 +358,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/worksheetdrawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
@@ -592,60 +614,37 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="3"/>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>49</v>
+      <c r="A2" s="3">
+        <v>0.9</v>
       </c>
       <c r="B2" s="3">
-        <v>0.0543</v>
+        <v>0.9</v>
       </c>
       <c r="C2" s="3">
-        <v>0.1711</v>
+        <v>0.9</v>
       </c>
       <c r="D2" s="3">
-        <v>3.0E-4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.009</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.3607</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.0085</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.2908</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.1048</v>
+        <v>0.9</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -662,30 +661,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>0.2258</v>
-      </c>
       <c r="B2" s="3">
-        <v>0.0705</v>
+        <v>0.0543</v>
       </c>
       <c r="C2" s="3">
-        <v>0.134</v>
+        <v>0.1711</v>
       </c>
       <c r="D2" s="3">
-        <v>0.5698</v>
+        <v>3.0E-4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.009</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.3607</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0085</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.2908</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.1048</v>
       </c>
     </row>
   </sheetData>
@@ -702,24 +730,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>40</v>
+        <v>53</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3">
-        <v>0.0198</v>
+        <v>0.2258</v>
       </c>
       <c r="B2" s="3">
-        <v>0.1032</v>
+        <v>0.0705</v>
       </c>
       <c r="C2" s="3">
-        <v>0.7419</v>
+        <v>0.134</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.5698</v>
       </c>
     </row>
   </sheetData>
@@ -736,156 +770,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>49</v>
+      <c r="A2" s="3">
+        <v>0.0198</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.1032</v>
       </c>
       <c r="C2" s="3">
-        <v>3.14</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1.73</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1.75</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1.75</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1.52</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1.52</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.0</v>
+        <v>0.7419</v>
       </c>
     </row>
   </sheetData>
@@ -905,22 +807,188 @@
         <v>55</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.14</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.73</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="B2" s="3">
         <v>1.0</v>
       </c>
@@ -973,7 +1041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1007,6 +1075,208 @@
       <c r="D2" s="1">
         <v>4.98</v>
       </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="33.86"/>
+    <col customWidth="1" min="2" max="2" width="15.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13">
+      <c r="B13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
change current coverage to zero
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -1106,7 +1106,7 @@
         <v>58</v>
       </c>
       <c r="B2" s="3">
-        <v>0.4</v>
+        <v>0.0</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="9"/>
@@ -1119,7 +1119,7 @@
         <v>59</v>
       </c>
       <c r="B3" s="3">
-        <v>0.5</v>
+        <v>0.0</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>

</xml_diff>

<commit_message>
added read intervention info from spreadsheet, started work on looping through interventions to increase coverage
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -21,7 +21,10 @@
     <sheet state="visible" name="RR birth by type" sheetId="16" r:id="rId18"/>
     <sheet state="visible" name="RR birth by time" sheetId="17" r:id="rId19"/>
     <sheet state="visible" name="OR birth outcome stunting" sheetId="18" r:id="rId20"/>
-    <sheet state="visible" name="Intervention coverages" sheetId="19" r:id="rId21"/>
+    <sheet state="visible" name="Interventions coverages" sheetId="19" r:id="rId21"/>
+    <sheet state="visible" name="Interventions affected fraction" sheetId="20" r:id="rId22"/>
+    <sheet state="visible" name="Interventions mortality eff" sheetId="21" r:id="rId23"/>
+    <sheet state="visible" name="Interventions incidence eff" sheetId="22" r:id="rId24"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -61,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="68">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -241,6 +244,30 @@
   </si>
   <si>
     <t>Vitamin A supplementation</t>
+  </si>
+  <si>
+    <t>Complementary feeding 1</t>
+  </si>
+  <si>
+    <t>Complementary feeding 2</t>
+  </si>
+  <si>
+    <t>Complementary feeding 3</t>
+  </si>
+  <si>
+    <t>Breastfeeding promotion</t>
+  </si>
+  <si>
+    <t>IPTp</t>
+  </si>
+  <si>
+    <t>BES</t>
+  </si>
+  <si>
+    <t>MMS</t>
+  </si>
+  <si>
+    <t>Interventions</t>
   </si>
 </sst>
 </file>
@@ -250,7 +277,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -264,6 +291,9 @@
     <font/>
     <font>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -285,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -314,6 +344,12 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -367,6 +403,18 @@
 </file>
 
 <file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/worksheetdrawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/worksheetdrawing21.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/worksheetdrawing22.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -1127,55 +1175,84 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.0</v>
+      </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
+      <c r="A5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.0</v>
+      </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.0</v>
+      </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.0</v>
+      </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.0</v>
+      </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.0</v>
+      </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10">
-      <c r="B10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.0</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1649,6 +1726,435 @@
       <c r="F18" s="2">
         <v>0.285</v>
       </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="12">
+        <v>0.253</v>
+      </c>
+      <c r="G2" s="12">
+        <v>0.253</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="12">
+        <v>0.253</v>
+      </c>
+      <c r="G3" s="12">
+        <v>0.253</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.416</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.416</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0.416</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
rename tabs, generalise stuff by intervention or condition
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -11,16 +11,16 @@
     <sheet state="visible" name="RRBreastfeeding" sheetId="6" r:id="rId8"/>
     <sheet state="visible" name="RR Death by Birth Outcome" sheetId="7" r:id="rId9"/>
     <sheet state="visible" name="OR stunting progression" sheetId="8" r:id="rId10"/>
-    <sheet state="visible" name="Incidence diarrhoea" sheetId="9" r:id="rId11"/>
+    <sheet state="visible" name="Incidence of conditions" sheetId="9" r:id="rId11"/>
     <sheet state="visible" name="RR diarrhoea" sheetId="10" r:id="rId12"/>
-    <sheet state="visible" name="OR stunting diarrhoea" sheetId="11" r:id="rId13"/>
-    <sheet state="visible" name="OR stunting Zinc" sheetId="12" r:id="rId14"/>
+    <sheet state="visible" name="OR stunting by condition" sheetId="11" r:id="rId13"/>
+    <sheet state="visible" name="OR stunting by intervention" sheetId="12" r:id="rId14"/>
     <sheet state="visible" name="birth distribution" sheetId="13" r:id="rId15"/>
     <sheet state="visible" name="time between births" sheetId="14" r:id="rId16"/>
     <sheet state="visible" name="birth outcome distribution" sheetId="15" r:id="rId17"/>
     <sheet state="visible" name="RR birth by type" sheetId="16" r:id="rId18"/>
     <sheet state="visible" name="RR birth by time" sheetId="17" r:id="rId19"/>
-    <sheet state="visible" name="OR birth outcome stunting" sheetId="18" r:id="rId20"/>
+    <sheet state="visible" name="OR stunting by birth outcome" sheetId="18" r:id="rId20"/>
     <sheet state="visible" name="Interventions coverages" sheetId="19" r:id="rId21"/>
     <sheet state="visible" name="Interventions affected fraction" sheetId="20" r:id="rId22"/>
     <sheet state="visible" name="Interventions mortality eff" sheetId="21" r:id="rId23"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="69">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -198,9 +198,18 @@
     <t>Neonatal congenital anomalies</t>
   </si>
   <si>
+    <t>Condition</t>
+  </si>
+  <si>
     <t>Breastfeeding Category</t>
   </si>
   <si>
+    <t>Intervention</t>
+  </si>
+  <si>
+    <t>Zinc supplementation</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -234,13 +243,7 @@
     <t>Outcome</t>
   </si>
   <si>
-    <t>Intervention</t>
-  </si>
-  <si>
     <t>pre-2016</t>
-  </si>
-  <si>
-    <t>Zinc supplementation</t>
   </si>
   <si>
     <t>Vitamin A supplementation</t>
@@ -508,7 +511,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -619,25 +622,28 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>1.04</v>
+      <c r="A2" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B2">
         <v>1.04</v>
@@ -649,6 +655,9 @@
         <v>1.04</v>
       </c>
       <c r="E2">
+        <v>1.04</v>
+      </c>
+      <c r="F2">
         <v>1.04</v>
       </c>
     </row>
@@ -663,38 +672,47 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="22.86"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4">
+      <c r="A2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="4">
         <v>0.9</v>
       </c>
-      <c r="B2" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>0.9</v>
       </c>
     </row>
@@ -712,22 +730,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B2" s="4">
         <v>0.0543</v>
@@ -741,7 +759,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B3" s="4">
         <v>0.009</v>
@@ -755,7 +773,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B4" s="4">
         <v>0.0</v>
@@ -781,16 +799,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2">
@@ -855,19 +873,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2">
@@ -875,7 +893,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C2" s="4">
         <v>3.14</v>
@@ -890,7 +908,7 @@
     <row r="3">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C3" s="4">
         <v>1.6</v>
@@ -905,7 +923,7 @@
     <row r="4">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C4" s="4">
         <v>1.6</v>
@@ -922,7 +940,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C5" s="4">
         <v>1.75</v>
@@ -936,7 +954,7 @@
     </row>
     <row r="6">
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C6" s="4">
         <v>1.4</v>
@@ -950,7 +968,7 @@
     </row>
     <row r="7">
       <c r="B7" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C7" s="4">
         <v>1.4</v>
@@ -967,7 +985,7 @@
         <v>40</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C8" s="4">
         <v>1.52</v>
@@ -981,7 +999,7 @@
     </row>
     <row r="9">
       <c r="B9" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C9" s="4">
         <v>1.2</v>
@@ -995,7 +1013,7 @@
     </row>
     <row r="10">
       <c r="B10" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C10" s="4">
         <v>1.2</v>
@@ -1021,19 +1039,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2">
@@ -1145,16 +1163,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B2" s="4">
         <v>0.0</v>
@@ -1167,7 +1185,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" s="4">
         <v>0.0</v>
@@ -1179,7 +1197,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" s="4">
         <v>0.0</v>
@@ -1191,7 +1209,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5" s="4">
         <v>0.0</v>
@@ -1203,7 +1221,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B6" s="4">
         <v>0.0</v>
@@ -1215,7 +1233,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B7" s="4">
         <v>0.0</v>
@@ -1227,7 +1245,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B8" s="4">
         <v>0.0</v>
@@ -1239,7 +1257,7 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B9" s="4">
         <v>0.0</v>
@@ -1251,7 +1269,7 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B10" s="4">
         <v>0.0</v>
@@ -1744,7 +1762,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -1767,7 +1785,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
@@ -1811,7 +1829,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -1884,10 +1902,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="17.29"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -1910,7 +1931,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
@@ -1954,7 +1975,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -2030,7 +2051,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -2053,7 +2074,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
@@ -2097,7 +2118,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -4305,37 +4326,63 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11">
-        <v>0.23981666666666668</v>
+      <c r="A2" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B2" s="11">
         <v>0.23981666666666668</v>
       </c>
       <c r="C2" s="11">
+        <v>0.23981666666666668</v>
+      </c>
+      <c r="D2" s="11">
         <v>0.36586416666666666</v>
       </c>
-      <c r="D2" s="11">
+      <c r="E2" s="11">
         <v>0.29612333333333335</v>
       </c>
-      <c r="E2" s="11">
+      <c r="F2" s="11">
         <v>0.18924083333333333</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added interventionsMaternal to spreadsheet and data
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -22,9 +22,10 @@
     <sheet state="visible" name="RR birth by time" sheetId="17" r:id="rId19"/>
     <sheet state="visible" name="OR stunting by birth outcome" sheetId="18" r:id="rId20"/>
     <sheet state="visible" name="Interventions coverages" sheetId="19" r:id="rId21"/>
-    <sheet state="visible" name="Interventions affected fraction" sheetId="20" r:id="rId22"/>
-    <sheet state="visible" name="Interventions mortality eff" sheetId="21" r:id="rId23"/>
-    <sheet state="visible" name="Interventions incidence eff" sheetId="22" r:id="rId24"/>
+    <sheet state="visible" name="Interventions maternal" sheetId="20" r:id="rId22"/>
+    <sheet state="visible" name="Interventions affected fraction" sheetId="21" r:id="rId23"/>
+    <sheet state="visible" name="Interventions mortality eff" sheetId="22" r:id="rId24"/>
+    <sheet state="visible" name="Interventions incidence eff" sheetId="23" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="71">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -264,10 +265,16 @@
     <t>IPTp</t>
   </si>
   <si>
-    <t>BES</t>
-  </si>
-  <si>
-    <t>MMS</t>
+    <t>Balanced energy supplementation</t>
+  </si>
+  <si>
+    <t>Multiple micronutrient supplementation</t>
+  </si>
+  <si>
+    <t>effectiveness</t>
+  </si>
+  <si>
+    <t>affected fraction</t>
   </si>
   <si>
     <t>Interventions</t>
@@ -318,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -350,6 +357,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
@@ -421,6 +429,10 @@
 </file>
 
 <file path=xl/drawings/worksheetdrawing22.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/worksheetdrawing23.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -1256,7 +1268,7 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
         <v>66</v>
       </c>
       <c r="B9" s="4">
@@ -1268,7 +1280,7 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="4">
@@ -1762,7 +1774,150 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
         <v>68</v>
+      </c>
+      <c r="C2" s="13">
+        <v>0.35</v>
+      </c>
+      <c r="D2" s="13">
+        <v>0.35</v>
+      </c>
+      <c r="E2" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0.31</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0.31</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0.336</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.336</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.336</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.09</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.09</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -1799,10 +1954,10 @@
       <c r="E2" s="4">
         <v>0.0</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="14">
         <v>0.253</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="14">
         <v>0.253</v>
       </c>
     </row>
@@ -1820,10 +1975,10 @@
       <c r="E3" s="4">
         <v>0.0</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="14">
         <v>0.253</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="14">
         <v>0.253</v>
       </c>
     </row>
@@ -1843,10 +1998,10 @@
       <c r="E4" s="4">
         <v>0.416</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="15">
         <v>0.416</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="15">
         <v>0.416</v>
       </c>
     </row>
@@ -1896,7 +2051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1908,7 +2063,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -2042,7 +2197,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2051,7 +2206,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
add coverage and effect of complementary feeding
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="71">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -211,6 +211,15 @@
     <t>Zinc supplementation</t>
   </si>
   <si>
+    <t>Complementary feeding (food secure without promotion)</t>
+  </si>
+  <si>
+    <t>Complementary feeding (food insecure with promotion and supplementation)</t>
+  </si>
+  <si>
+    <t>Complementary feeding (food insecure with neither promotion nor supplementation)</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -248,15 +257,6 @@
   </si>
   <si>
     <t>Vitamin A supplementation</t>
-  </si>
-  <si>
-    <t>Complementary feeding 1</t>
-  </si>
-  <si>
-    <t>Complementary feeding 2</t>
-  </si>
-  <si>
-    <t>Complementary feeding 3</t>
   </si>
   <si>
     <t>Breastfeeding promotion</t>
@@ -325,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -357,6 +357,9 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
@@ -685,7 +688,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.86"/>
+    <col customWidth="1" min="1" max="1" width="70.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -726,6 +729,66 @@
       </c>
       <c r="F2" s="4">
         <v>0.9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.43</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1.43</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2.39</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2.39</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -742,22 +805,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B2" s="4">
         <v>0.0543</v>
@@ -771,7 +834,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B3" s="4">
         <v>0.009</v>
@@ -785,7 +848,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4">
         <v>0.0</v>
@@ -811,16 +874,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2">
@@ -885,19 +948,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2">
@@ -905,7 +968,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C2" s="4">
         <v>3.14</v>
@@ -920,7 +983,7 @@
     <row r="3">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C3" s="4">
         <v>1.6</v>
@@ -935,7 +998,7 @@
     <row r="4">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C4" s="4">
         <v>1.6</v>
@@ -952,7 +1015,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C5" s="4">
         <v>1.75</v>
@@ -966,7 +1029,7 @@
     </row>
     <row r="6">
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C6" s="4">
         <v>1.4</v>
@@ -980,7 +1043,7 @@
     </row>
     <row r="7">
       <c r="B7" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C7" s="4">
         <v>1.4</v>
@@ -997,7 +1060,7 @@
         <v>40</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C8" s="4">
         <v>1.52</v>
@@ -1011,7 +1074,7 @@
     </row>
     <row r="9">
       <c r="B9" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C9" s="4">
         <v>1.2</v>
@@ -1025,7 +1088,7 @@
     </row>
     <row r="10">
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C10" s="4">
         <v>1.2</v>
@@ -1051,19 +1114,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2">
@@ -1169,7 +1232,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="33.86"/>
+    <col customWidth="1" min="1" max="1" width="52.57"/>
     <col customWidth="1" min="2" max="2" width="15.57"/>
   </cols>
   <sheetData>
@@ -1178,7 +1241,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C1" s="4"/>
     </row>
@@ -1186,7 +1249,7 @@
       <c r="A2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="13">
         <v>0.0</v>
       </c>
       <c r="C2" s="4"/>
@@ -1197,10 +1260,10 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B3" s="4">
-        <v>0.0</v>
+        <v>0.19</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -1209,10 +1272,10 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4">
-        <v>0.0</v>
+        <v>0.385</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -1221,10 +1284,10 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4">
-        <v>0.0</v>
+        <v>0.385</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -1233,10 +1296,10 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B6" s="4">
-        <v>0.0</v>
+        <v>0.385</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -1248,7 +1311,7 @@
         <v>64</v>
       </c>
       <c r="B7" s="4">
-        <v>0.0</v>
+        <v>0.296</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -1260,7 +1323,7 @@
         <v>65</v>
       </c>
       <c r="B8" s="4">
-        <v>0.0</v>
+        <v>0.257</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -1777,7 +1840,7 @@
         <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>42</v>
@@ -1799,16 +1862,16 @@
       <c r="B2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="14">
         <v>0.35</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="14">
         <v>0.35</v>
       </c>
-      <c r="E2" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="13">
+      <c r="E2" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="14">
         <v>0.0</v>
       </c>
     </row>
@@ -1816,16 +1879,16 @@
       <c r="B3" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="13">
+      <c r="C3" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="14">
         <v>0.0</v>
       </c>
     </row>
@@ -1836,16 +1899,16 @@
       <c r="B4" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="14">
         <v>0.31</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="14">
         <v>0.31</v>
       </c>
-      <c r="E4" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="13">
+      <c r="E4" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="14">
         <v>0.0</v>
       </c>
     </row>
@@ -1853,16 +1916,16 @@
       <c r="B5" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="14">
         <v>0.336</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="14">
         <v>0.336</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="14">
         <v>0.336</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="14">
         <v>0.0</v>
       </c>
     </row>
@@ -1873,16 +1936,16 @@
       <c r="B6" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="14">
         <v>0.09</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="14">
         <v>0.09</v>
       </c>
-      <c r="E6" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="13">
+      <c r="E6" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="14">
         <v>0.0</v>
       </c>
     </row>
@@ -1890,16 +1953,16 @@
       <c r="B7" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="13">
+      <c r="C7" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="14">
         <v>0.0</v>
       </c>
     </row>
@@ -1954,10 +2017,10 @@
       <c r="E2" s="4">
         <v>0.0</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="15">
         <v>0.253</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="15">
         <v>0.253</v>
       </c>
     </row>
@@ -1975,16 +2038,16 @@
       <c r="E3" s="4">
         <v>0.0</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="15">
         <v>0.253</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="15">
         <v>0.253</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -1998,10 +2061,10 @@
       <c r="E4" s="4">
         <v>0.416</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="16">
         <v>0.416</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="16">
         <v>0.416</v>
       </c>
     </row>
@@ -2130,7 +2193,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -2273,7 +2336,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
add breastfeeding promotion OR
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -15,17 +15,18 @@
     <sheet state="visible" name="RR diarrhoea" sheetId="10" r:id="rId12"/>
     <sheet state="visible" name="OR stunting by condition" sheetId="11" r:id="rId13"/>
     <sheet state="visible" name="OR stunting by intervention" sheetId="12" r:id="rId14"/>
-    <sheet state="visible" name="birth distribution" sheetId="13" r:id="rId15"/>
-    <sheet state="visible" name="time between births" sheetId="14" r:id="rId16"/>
-    <sheet state="visible" name="birth outcome distribution" sheetId="15" r:id="rId17"/>
-    <sheet state="visible" name="RR birth by type" sheetId="16" r:id="rId18"/>
-    <sheet state="visible" name="RR birth by time" sheetId="17" r:id="rId19"/>
-    <sheet state="visible" name="OR stunting by birth outcome" sheetId="18" r:id="rId20"/>
-    <sheet state="visible" name="Interventions coverages" sheetId="19" r:id="rId21"/>
-    <sheet state="visible" name="Interventions maternal" sheetId="20" r:id="rId22"/>
-    <sheet state="visible" name="Interventions affected fraction" sheetId="21" r:id="rId23"/>
-    <sheet state="visible" name="Interventions mortality eff" sheetId="22" r:id="rId24"/>
-    <sheet state="visible" name="Interventions incidence eff" sheetId="23" r:id="rId25"/>
+    <sheet state="visible" name="OR exclusive breastfeeding by p" sheetId="13" r:id="rId15"/>
+    <sheet state="visible" name="birth outcome distribution" sheetId="14" r:id="rId16"/>
+    <sheet state="visible" name="OR stunting by birth outcome" sheetId="15" r:id="rId17"/>
+    <sheet state="visible" name="Interventions coverages" sheetId="16" r:id="rId18"/>
+    <sheet state="visible" name="Interventions maternal" sheetId="17" r:id="rId19"/>
+    <sheet state="visible" name="Interventions affected fraction" sheetId="18" r:id="rId20"/>
+    <sheet state="visible" name="Interventions mortality eff" sheetId="19" r:id="rId21"/>
+    <sheet state="visible" name="Interventions incidence eff" sheetId="20" r:id="rId22"/>
+    <sheet state="visible" name="RR birth by type" sheetId="21" r:id="rId23"/>
+    <sheet state="visible" name="birth distribution" sheetId="22" r:id="rId24"/>
+    <sheet state="visible" name="time between births" sheetId="23" r:id="rId25"/>
+    <sheet state="visible" name="RR birth by time" sheetId="24" r:id="rId26"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="72">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -220,6 +221,39 @@
     <t>Complementary feeding (food insecure with neither promotion nor supplementation)</t>
   </si>
   <si>
+    <t>Breastfeeding promotion - Health system</t>
+  </si>
+  <si>
+    <t>Breastfeeding promotion - Home/community</t>
+  </si>
+  <si>
+    <t>pre-2016</t>
+  </si>
+  <si>
+    <t>Vitamin A supplementation</t>
+  </si>
+  <si>
+    <t>IPTp</t>
+  </si>
+  <si>
+    <t>Balanced energy supplementation</t>
+  </si>
+  <si>
+    <t>Multiple micronutrient supplementation</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>effectiveness</t>
+  </si>
+  <si>
+    <t>affected fraction</t>
+  </si>
+  <si>
+    <t>Interventions</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -248,36 +282,6 @@
   </si>
   <si>
     <t>&lt;24 months</t>
-  </si>
-  <si>
-    <t>Outcome</t>
-  </si>
-  <si>
-    <t>pre-2016</t>
-  </si>
-  <si>
-    <t>Vitamin A supplementation</t>
-  </si>
-  <si>
-    <t>Breastfeeding promotion</t>
-  </si>
-  <si>
-    <t>IPTp</t>
-  </si>
-  <si>
-    <t>Balanced energy supplementation</t>
-  </si>
-  <si>
-    <t>Multiple micronutrient supplementation</t>
-  </si>
-  <si>
-    <t>effectiveness</t>
-  </si>
-  <si>
-    <t>affected fraction</t>
-  </si>
-  <si>
-    <t>Interventions</t>
   </si>
 </sst>
 </file>
@@ -325,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -355,6 +359,12 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -439,6 +449,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing24.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
@@ -802,63 +816,89 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="37.29"/>
+    <col customWidth="1" min="2" max="2" width="10.71"/>
+    <col customWidth="1" min="3" max="3" width="12.71"/>
+    <col customWidth="1" min="4" max="4" width="11.14"/>
+    <col customWidth="1" min="5" max="6" width="12.29"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.0543</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.1711</v>
-      </c>
-      <c r="D2" s="4">
-        <v>3.0E-4</v>
+        <v>51</v>
+      </c>
+      <c r="B2" s="12">
+        <v>2.3</v>
+      </c>
+      <c r="C2" s="12">
+        <v>4.6</v>
+      </c>
+      <c r="D2" s="12">
+        <v>1.57</v>
+      </c>
+      <c r="E2" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.009</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.3607</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.0085</v>
+        <v>52</v>
+      </c>
+      <c r="B3" s="12">
+        <v>2.3</v>
+      </c>
+      <c r="C3" s="12">
+        <v>4.6</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1.57</v>
+      </c>
+      <c r="E3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="13">
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.2908</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.1048</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -874,30 +914,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4">
-        <v>0.2258</v>
+        <v>0.0198</v>
       </c>
       <c r="B2" s="4">
-        <v>0.0705</v>
+        <v>0.1032</v>
       </c>
       <c r="C2" s="4">
-        <v>0.134</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.5698</v>
+        <v>0.7419</v>
       </c>
     </row>
   </sheetData>
@@ -913,25 +947,31 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="4">
-        <v>0.0198</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.1032</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.7419</v>
+      <c r="A2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.82</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.94</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.98</v>
       </c>
     </row>
   </sheetData>
@@ -945,160 +985,237 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="57.57"/>
+    <col customWidth="1" min="2" max="2" width="15.57"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="C1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="4">
-        <v>3.14</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1.73</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1.73</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1.57</v>
-      </c>
+      <c r="A3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1.57</v>
-      </c>
+      <c r="A4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.385</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1.75</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1.75</v>
-      </c>
-      <c r="E5" s="4">
-        <v>1.75</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.385</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6">
-      <c r="B6" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>1.33</v>
-      </c>
+      <c r="A6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.385</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7">
-      <c r="B7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1.33</v>
-      </c>
+      <c r="A7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.196</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="4">
-        <v>1.52</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1.52</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="4">
+        <v>0.257</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1.0</v>
-      </c>
+      <c r="B11" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13">
+      <c r="B13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1111,73 +1228,139 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="30.14"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="B2" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="C2" s="16">
+        <v>0.35</v>
+      </c>
+      <c r="D2" s="16">
+        <v>0.35</v>
+      </c>
+      <c r="E2" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>3.03</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1.77</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1.49</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1.1</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1.0</v>
+      <c r="C3" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1.41</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1.18</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1.0</v>
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0.31</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0.31</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0.336</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0.336</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0.336</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.09</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.09</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -1191,34 +1374,140 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="25.71"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>42</v>
+      <c r="A1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2.82</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.94</v>
-      </c>
-      <c r="D2" s="1">
-        <v>4.98</v>
-      </c>
+      <c r="A2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0.253</v>
+      </c>
+      <c r="G2" s="17">
+        <v>0.253</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0.253</v>
+      </c>
+      <c r="G3" s="17">
+        <v>0.253</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.416</v>
+      </c>
+      <c r="F4" s="18">
+        <v>0.416</v>
+      </c>
+      <c r="G4" s="18">
+        <v>0.416</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1232,224 +1521,139 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="52.57"/>
-    <col customWidth="1" min="2" max="2" width="15.57"/>
+    <col customWidth="1" min="1" max="1" width="25.29"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.19</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.51</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.51</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0.385</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0.385</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0.385</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0.296</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0.257</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11">
-      <c r="B11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15">
-      <c r="B15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16">
-      <c r="B16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17">
-      <c r="B17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-    </row>
-    <row r="22">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1837,134 +2041,134 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" t="s">
         <v>61</v>
       </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>39</v>
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="14">
-        <v>0.35</v>
-      </c>
-      <c r="D2" s="14">
-        <v>0.35</v>
-      </c>
-      <c r="E2" s="14">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="14">
-        <v>0.0</v>
+      <c r="A2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.65</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="14">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="14">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="14">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="14">
-        <v>0.0</v>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.52</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="14">
-        <v>0.31</v>
-      </c>
-      <c r="D4" s="14">
-        <v>0.31</v>
-      </c>
-      <c r="E4" s="14">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="14">
-        <v>0.0</v>
+      <c r="A4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.62</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="14">
-        <v>0.336</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0.336</v>
-      </c>
-      <c r="E5" s="14">
-        <v>0.336</v>
-      </c>
-      <c r="F5" s="14">
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="4">
         <v>0.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="14">
-        <v>0.09</v>
-      </c>
-      <c r="D6" s="14">
-        <v>0.09</v>
-      </c>
-      <c r="E6" s="14">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="14">
-        <v>0.0</v>
-      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7">
-      <c r="B7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="14">
-        <v>0.0</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1980,134 +2184,157 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
+        <v>62</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="C2" s="4">
-        <v>0.0</v>
+        <v>3.14</v>
       </c>
       <c r="D2" s="4">
-        <v>0.0</v>
+        <v>1.73</v>
       </c>
       <c r="E2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="15">
-        <v>0.253</v>
-      </c>
-      <c r="G2" s="15">
-        <v>0.253</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="C3" s="4">
-        <v>0.0</v>
+        <v>1.6</v>
       </c>
       <c r="D3" s="4">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="15">
-        <v>0.253</v>
-      </c>
-      <c r="G3" s="15">
-        <v>0.253</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="C4" s="4">
-        <v>0.0</v>
+        <v>1.6</v>
       </c>
       <c r="D4" s="4">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E4" s="4">
-        <v>0.416</v>
-      </c>
-      <c r="F4" s="16">
-        <v>0.416</v>
-      </c>
-      <c r="G4" s="16">
-        <v>0.416</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="C5" s="4">
-        <v>0.0</v>
+        <v>1.75</v>
       </c>
       <c r="D5" s="4">
-        <v>0.0</v>
+        <v>1.75</v>
       </c>
       <c r="E5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.0</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.33</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.33</v>
+      </c>
     </row>
     <row r="8">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1.52</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.52</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.52</v>
+      </c>
     </row>
     <row r="9">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2120,140 +2347,63 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="17.29"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>66</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.0543</v>
       </c>
       <c r="C2" s="4">
-        <v>0.0</v>
+        <v>0.1711</v>
       </c>
       <c r="D2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0.5</v>
+        <v>3.0E-4</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
+      <c r="A3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.009</v>
       </c>
       <c r="C3" s="4">
-        <v>0.0</v>
+        <v>0.3607</v>
       </c>
       <c r="D3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.51</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.51</v>
+        <v>0.0085</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>68</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.0</v>
       </c>
       <c r="C4" s="4">
-        <v>0.0</v>
+        <v>0.2908</v>
       </c>
       <c r="D4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+        <v>0.1048</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2269,134 +2419,111 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4">
+        <v>0.2258</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.0705</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.134</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.5698</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
+        <v>66</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>42</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1.0</v>
       </c>
       <c r="C2" s="4">
-        <v>0.0</v>
+        <v>3.03</v>
       </c>
       <c r="D2" s="4">
-        <v>0.0</v>
+        <v>1.77</v>
       </c>
       <c r="E2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0.65</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
+      <c r="A3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1.0</v>
       </c>
       <c r="C3" s="4">
-        <v>0.0</v>
+        <v>1.49</v>
       </c>
       <c r="D3" s="4">
-        <v>0.0</v>
+        <v>1.1</v>
       </c>
       <c r="E3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.52</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.52</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>40</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1.0</v>
       </c>
       <c r="C4" s="4">
-        <v>0.0</v>
+        <v>1.41</v>
       </c>
       <c r="D4" s="4">
-        <v>0.0</v>
+        <v>1.18</v>
       </c>
       <c r="E4" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+        <v>1.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
split ORstunting for Zinc and Complementary feeding
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -14,19 +14,20 @@
     <sheet state="visible" name="Incidence of conditions" sheetId="9" r:id="rId11"/>
     <sheet state="visible" name="RR diarrhoea" sheetId="10" r:id="rId12"/>
     <sheet state="visible" name="OR stunting by condition" sheetId="11" r:id="rId13"/>
-    <sheet state="visible" name="OR stunting by intervention" sheetId="12" r:id="rId14"/>
-    <sheet state="visible" name="OR exclusive breastfeeding by p" sheetId="13" r:id="rId15"/>
-    <sheet state="visible" name="birth outcome distribution" sheetId="14" r:id="rId16"/>
-    <sheet state="visible" name="OR stunting by birth outcome" sheetId="15" r:id="rId17"/>
-    <sheet state="visible" name="Interventions coverages" sheetId="16" r:id="rId18"/>
-    <sheet state="visible" name="Interventions maternal" sheetId="17" r:id="rId19"/>
-    <sheet state="visible" name="Interventions affected fraction" sheetId="18" r:id="rId20"/>
-    <sheet state="visible" name="Interventions mortality eff" sheetId="19" r:id="rId21"/>
-    <sheet state="visible" name="Interventions incidence eff" sheetId="20" r:id="rId22"/>
-    <sheet state="visible" name="RR birth by type" sheetId="21" r:id="rId23"/>
-    <sheet state="visible" name="birth distribution" sheetId="22" r:id="rId24"/>
-    <sheet state="visible" name="time between births" sheetId="23" r:id="rId25"/>
-    <sheet state="visible" name="RR birth by time" sheetId="24" r:id="rId26"/>
+    <sheet state="visible" name="birth outcome distribution" sheetId="12" r:id="rId14"/>
+    <sheet state="visible" name="OR stunting by birth outcome" sheetId="13" r:id="rId15"/>
+    <sheet state="visible" name="OR stunting by intervention" sheetId="14" r:id="rId16"/>
+    <sheet state="visible" name="OR stunting for complementary f" sheetId="15" r:id="rId17"/>
+    <sheet state="visible" name="OR exclusive breastfeeding by p" sheetId="16" r:id="rId18"/>
+    <sheet state="visible" name="Interventions coverages" sheetId="17" r:id="rId19"/>
+    <sheet state="visible" name="Interventions maternal" sheetId="18" r:id="rId20"/>
+    <sheet state="visible" name="Interventions affected fraction" sheetId="19" r:id="rId21"/>
+    <sheet state="visible" name="Interventions mortality eff" sheetId="20" r:id="rId22"/>
+    <sheet state="visible" name="Interventions incidence eff" sheetId="21" r:id="rId23"/>
+    <sheet state="visible" name="RR birth by type" sheetId="22" r:id="rId24"/>
+    <sheet state="visible" name="birth distribution" sheetId="23" r:id="rId25"/>
+    <sheet state="visible" name="time between births" sheetId="24" r:id="rId26"/>
+    <sheet state="visible" name="RR birth by time" sheetId="25" r:id="rId27"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="74">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -212,6 +213,9 @@
     <t>Zinc supplementation</t>
   </si>
   <si>
+    <t>Complementary feeding (food secure with promotion)</t>
+  </si>
+  <si>
     <t>Complementary feeding (food secure without promotion)</t>
   </si>
   <si>
@@ -231,6 +235,9 @@
   </si>
   <si>
     <t>Vitamin A supplementation</t>
+  </si>
+  <si>
+    <t>Complementary feeding (promotion and supplementation if needed)</t>
   </si>
   <si>
     <t>IPTp</t>
@@ -359,13 +366,13 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
@@ -453,6 +460,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing25.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
@@ -701,6 +712,80 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4">
+        <v>0.0198</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.1032</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.7419</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.82</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.94</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.98</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="70.86"/>
   </cols>
@@ -746,71 +831,148 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1.43</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1.43</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1.0</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1.0</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>2.39</v>
-      </c>
-      <c r="E5" s="4">
-        <v>2.39</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1.0</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="70.86"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4"/>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.43</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1.43</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2.39</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2.39</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -846,41 +1008,41 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="12">
+        <v>52</v>
+      </c>
+      <c r="B2" s="13">
         <v>2.3</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="13">
         <v>4.6</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="13">
         <v>1.57</v>
       </c>
-      <c r="E2" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="F2" s="13">
+      <c r="E2" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="F2" s="14">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="12">
+        <v>53</v>
+      </c>
+      <c r="B3" s="13">
         <v>2.3</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="13">
         <v>4.6</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="13">
         <v>1.57</v>
       </c>
-      <c r="E3" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="13">
+      <c r="E3" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="14">
         <v>1.0</v>
       </c>
     </row>
@@ -905,81 +1067,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4">
-        <v>0.0198</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.1032</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.7419</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2.82</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.94</v>
-      </c>
-      <c r="D2" s="1">
-        <v>4.98</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -995,7 +1083,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C1" s="4"/>
     </row>
@@ -1014,7 +1102,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4">
         <v>0.19</v>
@@ -1026,7 +1114,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4">
         <v>0.385</v>
@@ -1038,10 +1126,10 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B5" s="4">
-        <v>0.385</v>
+        <v>0.196</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -1050,10 +1138,10 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B6" s="4">
-        <v>0.385</v>
+        <v>0.1</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -1062,10 +1150,10 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B7" s="4">
-        <v>0.196</v>
+        <v>0.257</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -1073,11 +1161,11 @@
       <c r="G7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>52</v>
+      <c r="A8" t="s">
+        <v>58</v>
       </c>
       <c r="B8" s="4">
-        <v>0.1</v>
+        <v>0.0</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -1085,36 +1173,26 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>55</v>
+      <c r="A9" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="B9" s="4">
-        <v>0.257</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+        <v>0.0</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="B10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0.0</v>
-      </c>
+      <c r="B11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1157,17 +1235,11 @@
     </row>
     <row r="17">
       <c r="B17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="C17" s="4"/>
     </row>
     <row r="18">
       <c r="B18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="C18" s="4"/>
     </row>
     <row r="19">
       <c r="B19" s="4"/>
@@ -1209,20 +1281,12 @@
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="29">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1237,7 +1301,7 @@
         <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
         <v>42</v>
@@ -1254,10 +1318,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C2" s="16">
         <v>0.35</v>
@@ -1274,7 +1338,7 @@
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C3" s="16">
         <v>0.0</v>
@@ -1291,10 +1355,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C4" s="16">
         <v>0.31</v>
@@ -1311,7 +1375,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C5" s="16">
         <v>0.336</v>
@@ -1328,10 +1392,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C6" s="16">
         <v>0.09</v>
@@ -1348,7 +1412,7 @@
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C7" s="16">
         <v>1.0</v>
@@ -1368,7 +1432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1380,7 +1444,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -1447,7 +1511,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -1514,7 +1578,379 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.003996</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.15484515</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.06893107</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.30969031</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.25974026</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.00899101</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.13186813</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.06193806</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.131</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.131</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.131</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.131</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.203</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.203</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.203</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.203</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.006</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.006</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.006</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.006</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.09300000000000001</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.09300000000000001</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.09300000000000001</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.09300000000000001</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.034</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.034</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.034</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.102</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.102</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.102</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.102</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.11599999999999999</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.11599999999999999</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.11599999999999999</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.11599999999999999</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.285</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.285</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.285</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.285</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1526,7 +1962,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -1593,7 +2029,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -1612,521 +2048,6 @@
       </c>
       <c r="G4" s="4">
         <v>0.3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.003996</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.15484515</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.06893107</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0.30969031</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.25974026</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.00899101</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.13186813</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.06193806</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.131</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.131</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.131</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.131</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.203</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.203</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.203</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.203</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0.03</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0.03</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0.03</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.006</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.006</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.006</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0.006</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.09300000000000001</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.09300000000000001</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.09300000000000001</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.09300000000000001</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0.034</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.034</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.034</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.034</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0.102</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.102</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0.102</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0.102</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0.11599999999999999</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.11599999999999999</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0.11599999999999999</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0.11599999999999999</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0.285</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.285</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0.285</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.285</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.52</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.62</v>
       </c>
     </row>
     <row r="5">
@@ -2184,157 +2105,134 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>65</v>
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="C2" s="4">
-        <v>3.14</v>
+        <v>0.0</v>
       </c>
       <c r="D2" s="4">
-        <v>1.73</v>
+        <v>0.0</v>
       </c>
       <c r="E2" s="4">
-        <v>1.73</v>
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.65</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4">
-        <v>1.6</v>
+        <v>0.0</v>
       </c>
       <c r="D3" s="4">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E3" s="4">
-        <v>1.57</v>
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.52</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="B4" s="4" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4">
-        <v>1.6</v>
+        <v>0.0</v>
       </c>
       <c r="D4" s="4">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E4" s="4">
-        <v>1.57</v>
+        <v>0.62</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.62</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="B5" s="4" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4">
-        <v>1.75</v>
+        <v>0.0</v>
       </c>
       <c r="D5" s="4">
-        <v>1.75</v>
+        <v>0.0</v>
       </c>
       <c r="E5" s="4">
-        <v>1.75</v>
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>1.33</v>
-      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7">
-      <c r="B7" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1.33</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1.52</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1.52</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1.52</v>
-      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9">
-      <c r="B9" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1.0</v>
-      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2350,59 +2248,156 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.0543</v>
+        <v>42</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="C2" s="4">
-        <v>0.1711</v>
+        <v>3.14</v>
       </c>
       <c r="D2" s="4">
-        <v>3.0E-4</v>
+        <v>1.73</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1.73</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.009</v>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="C3" s="4">
-        <v>0.3607</v>
+        <v>1.6</v>
       </c>
       <c r="D3" s="4">
-        <v>0.0085</v>
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1.57</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.2908</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.1048</v>
+      <c r="C5" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1.52</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.52</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -2419,30 +2414,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.0543</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.1711</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3.0E-4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B3" s="4">
+        <v>0.009</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.3607</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.0085</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4">
-        <v>0.2258</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.0705</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.134</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.5698</v>
+      <c r="B4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.2908</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.1048</v>
       </c>
     </row>
   </sheetData>
@@ -2459,19 +2483,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4">
+        <v>0.2258</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.0705</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.134</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.5698</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
shorten names of tabs
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -6,19 +6,19 @@
     <sheet state="visible" name="total mortality" sheetId="1" r:id="rId3"/>
     <sheet state="visible" name="mortality" sheetId="2" r:id="rId4"/>
     <sheet state="visible" name="distributions" sheetId="3" r:id="rId5"/>
-    <sheet state="visible" name="RRStunting" sheetId="4" r:id="rId6"/>
-    <sheet state="visible" name="RRWasting" sheetId="5" r:id="rId7"/>
-    <sheet state="visible" name="RRBreastfeeding" sheetId="6" r:id="rId8"/>
-    <sheet state="visible" name="RR Death by Birth Outcome" sheetId="7" r:id="rId9"/>
-    <sheet state="visible" name="OR stunting progression" sheetId="8" r:id="rId10"/>
-    <sheet state="visible" name="Incidence of conditions" sheetId="9" r:id="rId11"/>
-    <sheet state="visible" name="RR diarrhoea" sheetId="10" r:id="rId12"/>
-    <sheet state="visible" name="OR stunting by condition" sheetId="11" r:id="rId13"/>
-    <sheet state="visible" name="birth outcome distribution" sheetId="12" r:id="rId14"/>
+    <sheet state="visible" name="birth outcome distribution" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="RRStunting" sheetId="5" r:id="rId7"/>
+    <sheet state="visible" name="RRWasting" sheetId="6" r:id="rId8"/>
+    <sheet state="visible" name="RRBreastfeeding" sheetId="7" r:id="rId9"/>
+    <sheet state="visible" name="RR Death by Birth Outcome" sheetId="8" r:id="rId10"/>
+    <sheet state="visible" name="OR stunting progression" sheetId="9" r:id="rId11"/>
+    <sheet state="visible" name="Incidence of conditions" sheetId="10" r:id="rId12"/>
+    <sheet state="visible" name="RR diarrhoea" sheetId="11" r:id="rId13"/>
+    <sheet state="visible" name="OR stunting by condition" sheetId="12" r:id="rId14"/>
     <sheet state="visible" name="OR stunting by birth outcome" sheetId="13" r:id="rId15"/>
     <sheet state="visible" name="OR stunting by intervention" sheetId="14" r:id="rId16"/>
-    <sheet state="visible" name="OR stunting for complementary f" sheetId="15" r:id="rId17"/>
-    <sheet state="visible" name="OR exclusive breastfeeding by p" sheetId="16" r:id="rId18"/>
+    <sheet state="visible" name="OR stunting for complements" sheetId="15" r:id="rId17"/>
+    <sheet state="visible" name="OR exclusiveBF by intervention" sheetId="16" r:id="rId18"/>
     <sheet state="visible" name="Interventions coverages" sheetId="17" r:id="rId19"/>
     <sheet state="visible" name="Interventions maternal" sheetId="18" r:id="rId20"/>
     <sheet state="visible" name="Interventions affected fraction" sheetId="19" r:id="rId21"/>
@@ -177,6 +177,15 @@
     <t>none</t>
   </si>
   <si>
+    <t>Pre-term SGA</t>
+  </si>
+  <si>
+    <t>Pre-term AGA</t>
+  </si>
+  <si>
+    <t>Term SGA</t>
+  </si>
+  <si>
     <t>Stunting Status</t>
   </si>
   <si>
@@ -187,15 +196,6 @@
   </si>
   <si>
     <t>Term AGA</t>
-  </si>
-  <si>
-    <t>Term SGA</t>
-  </si>
-  <si>
-    <t>Pre-term AGA</t>
-  </si>
-  <si>
-    <t>Pre-term SGA</t>
   </si>
   <si>
     <t>Neonatal congenital anomalies</t>
@@ -545,6 +545,78 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0.23981666666666668</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0.23981666666666668</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0.36586416666666666</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0.29612333333333335</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.18924083333333333</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="25.86"/>
   </cols>
@@ -654,7 +726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -706,40 +778,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4">
-        <v>0.0198</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.1032</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.7419</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
@@ -749,16 +787,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
@@ -1304,16 +1342,16 @@
         <v>60</v>
       </c>
       <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2">
@@ -2265,7 +2303,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>68</v>
@@ -2312,7 +2350,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>68</v>
@@ -2357,7 +2395,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>68</v>
@@ -2540,7 +2578,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4">
         <v>1.0</v>
@@ -2557,7 +2595,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4">
         <v>1.0</v>
@@ -2574,7 +2612,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="4">
         <v>1.0</v>
@@ -2888,440 +2926,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
+        <v>37</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>26</v>
+      <c r="A2" s="4">
+        <v>0.0198</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.1032</v>
       </c>
       <c r="C2" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D2">
-        <v>1.0</v>
-      </c>
-      <c r="E2">
-        <v>1.0</v>
-      </c>
-      <c r="F2">
-        <v>1.0</v>
-      </c>
-      <c r="G2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D3">
-        <v>1.67</v>
-      </c>
-      <c r="E3">
-        <v>1.67</v>
-      </c>
-      <c r="F3">
-        <v>1.67</v>
-      </c>
-      <c r="G3">
-        <v>1.67</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D4">
-        <v>2.38</v>
-      </c>
-      <c r="E4">
-        <v>2.38</v>
-      </c>
-      <c r="F4">
-        <v>2.38</v>
-      </c>
-      <c r="G4">
-        <v>2.38</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D5">
-        <v>6.33</v>
-      </c>
-      <c r="E5">
-        <v>6.33</v>
-      </c>
-      <c r="F5">
-        <v>6.33</v>
-      </c>
-      <c r="G5">
-        <v>6.33</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D6">
-        <v>1.0</v>
-      </c>
-      <c r="E6">
-        <v>1.0</v>
-      </c>
-      <c r="F6">
-        <v>1.0</v>
-      </c>
-      <c r="G6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D7">
-        <v>1.55</v>
-      </c>
-      <c r="E7">
-        <v>1.55</v>
-      </c>
-      <c r="F7">
-        <v>1.55</v>
-      </c>
-      <c r="G7">
-        <v>1.55</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D8">
-        <v>2.18</v>
-      </c>
-      <c r="E8">
-        <v>2.18</v>
-      </c>
-      <c r="F8">
-        <v>2.18</v>
-      </c>
-      <c r="G8">
-        <v>2.18</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D9">
-        <v>6.39</v>
-      </c>
-      <c r="E9">
-        <v>6.39</v>
-      </c>
-      <c r="F9">
-        <v>6.39</v>
-      </c>
-      <c r="G9">
-        <v>6.39</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D10">
-        <v>1.0</v>
-      </c>
-      <c r="E10">
-        <v>1.0</v>
-      </c>
-      <c r="F10">
-        <v>1.0</v>
-      </c>
-      <c r="G10">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D11">
-        <v>1.0</v>
-      </c>
-      <c r="E11">
-        <v>1.0</v>
-      </c>
-      <c r="F11">
-        <v>1.0</v>
-      </c>
-      <c r="G11">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D12">
-        <v>2.79</v>
-      </c>
-      <c r="E12">
-        <v>2.79</v>
-      </c>
-      <c r="F12">
-        <v>2.79</v>
-      </c>
-      <c r="G12">
-        <v>2.79</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D13">
-        <v>6.01</v>
-      </c>
-      <c r="E13">
-        <v>6.01</v>
-      </c>
-      <c r="F13">
-        <v>6.01</v>
-      </c>
-      <c r="G13">
-        <v>6.01</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D14">
-        <v>1.0</v>
-      </c>
-      <c r="E14">
-        <v>1.0</v>
-      </c>
-      <c r="F14">
-        <v>1.0</v>
-      </c>
-      <c r="G14">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D15">
-        <v>1.0</v>
-      </c>
-      <c r="E15">
-        <v>1.0</v>
-      </c>
-      <c r="F15">
-        <v>1.0</v>
-      </c>
-      <c r="G15">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D16">
-        <v>1.0</v>
-      </c>
-      <c r="E16">
-        <v>1.0</v>
-      </c>
-      <c r="F16">
-        <v>1.0</v>
-      </c>
-      <c r="G16">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D17">
-        <v>1.0</v>
-      </c>
-      <c r="E17">
-        <v>1.0</v>
-      </c>
-      <c r="F17">
-        <v>1.0</v>
-      </c>
-      <c r="G17">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D18">
-        <v>1.0</v>
-      </c>
-      <c r="E18">
-        <v>1.0</v>
-      </c>
-      <c r="F18">
-        <v>1.0</v>
-      </c>
-      <c r="G18">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D19">
-        <v>1.0</v>
-      </c>
-      <c r="E19">
-        <v>1.0</v>
-      </c>
-      <c r="F19">
-        <v>1.0</v>
-      </c>
-      <c r="G19">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D20">
-        <v>1.86</v>
-      </c>
-      <c r="E20">
-        <v>1.86</v>
-      </c>
-      <c r="F20">
-        <v>1.86</v>
-      </c>
-      <c r="G20">
-        <v>1.86</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D21">
-        <v>3.01</v>
-      </c>
-      <c r="E21">
-        <v>3.01</v>
-      </c>
-      <c r="F21">
-        <v>3.01</v>
-      </c>
-      <c r="G21">
-        <v>3.01</v>
+        <v>0.7419</v>
       </c>
     </row>
   </sheetData>
@@ -3341,7 +2963,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -3390,16 +3012,16 @@
         <v>1.0</v>
       </c>
       <c r="D3">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
       <c r="E3">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
       <c r="F3">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
       <c r="G3">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="4">
@@ -3410,16 +3032,16 @@
         <v>1.0</v>
       </c>
       <c r="D4">
-        <v>3.41</v>
+        <v>2.38</v>
       </c>
       <c r="E4">
-        <v>3.41</v>
+        <v>2.38</v>
       </c>
       <c r="F4">
-        <v>3.41</v>
+        <v>2.38</v>
       </c>
       <c r="G4">
-        <v>3.41</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="5">
@@ -3430,16 +3052,16 @@
         <v>1.0</v>
       </c>
       <c r="D5">
-        <v>12.33</v>
+        <v>6.33</v>
       </c>
       <c r="E5">
-        <v>12.33</v>
+        <v>6.33</v>
       </c>
       <c r="F5">
-        <v>12.33</v>
+        <v>6.33</v>
       </c>
       <c r="G5">
-        <v>12.33</v>
+        <v>6.33</v>
       </c>
     </row>
     <row r="6">
@@ -3473,16 +3095,16 @@
         <v>1.0</v>
       </c>
       <c r="D7">
-        <v>1.92</v>
+        <v>1.55</v>
       </c>
       <c r="E7">
-        <v>1.92</v>
+        <v>1.55</v>
       </c>
       <c r="F7">
-        <v>1.92</v>
+        <v>1.55</v>
       </c>
       <c r="G7">
-        <v>1.92</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="8">
@@ -3493,16 +3115,16 @@
         <v>1.0</v>
       </c>
       <c r="D8">
-        <v>4.66</v>
+        <v>2.18</v>
       </c>
       <c r="E8">
-        <v>4.66</v>
+        <v>2.18</v>
       </c>
       <c r="F8">
-        <v>4.66</v>
+        <v>2.18</v>
       </c>
       <c r="G8">
-        <v>4.66</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="9">
@@ -3513,16 +3135,16 @@
         <v>1.0</v>
       </c>
       <c r="D9">
-        <v>9.68</v>
+        <v>6.39</v>
       </c>
       <c r="E9">
-        <v>9.68</v>
+        <v>6.39</v>
       </c>
       <c r="F9">
-        <v>9.68</v>
+        <v>6.39</v>
       </c>
       <c r="G9">
-        <v>9.68</v>
+        <v>6.39</v>
       </c>
     </row>
     <row r="10">
@@ -3576,16 +3198,16 @@
         <v>1.0</v>
       </c>
       <c r="D12">
-        <v>2.58</v>
+        <v>2.79</v>
       </c>
       <c r="E12">
-        <v>2.58</v>
+        <v>2.79</v>
       </c>
       <c r="F12">
-        <v>2.58</v>
+        <v>2.79</v>
       </c>
       <c r="G12">
-        <v>2.58</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="13">
@@ -3596,16 +3218,16 @@
         <v>1.0</v>
       </c>
       <c r="D13">
-        <v>9.63</v>
+        <v>6.01</v>
       </c>
       <c r="E13">
-        <v>9.63</v>
+        <v>6.01</v>
       </c>
       <c r="F13">
-        <v>9.63</v>
+        <v>6.01</v>
       </c>
       <c r="G13">
-        <v>9.63</v>
+        <v>6.01</v>
       </c>
     </row>
     <row r="14">
@@ -3722,16 +3344,16 @@
         <v>1.0</v>
       </c>
       <c r="D19">
-        <v>1.65</v>
+        <v>1.0</v>
       </c>
       <c r="E19">
-        <v>1.65</v>
+        <v>1.0</v>
       </c>
       <c r="F19">
-        <v>1.65</v>
+        <v>1.0</v>
       </c>
       <c r="G19">
-        <v>1.65</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="20">
@@ -3742,16 +3364,16 @@
         <v>1.0</v>
       </c>
       <c r="D20">
-        <v>2.73</v>
+        <v>1.86</v>
       </c>
       <c r="E20">
-        <v>2.73</v>
+        <v>1.86</v>
       </c>
       <c r="F20">
-        <v>2.73</v>
+        <v>1.86</v>
       </c>
       <c r="G20">
-        <v>2.73</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="21">
@@ -3762,16 +3384,16 @@
         <v>1.0</v>
       </c>
       <c r="D21">
-        <v>11.21</v>
+        <v>3.01</v>
       </c>
       <c r="E21">
-        <v>11.21</v>
+        <v>3.01</v>
       </c>
       <c r="F21">
-        <v>11.21</v>
+        <v>3.01</v>
       </c>
       <c r="G21">
-        <v>11.21</v>
+        <v>3.01</v>
       </c>
     </row>
   </sheetData>
@@ -3780,6 +3402,456 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D2">
+        <v>1.0</v>
+      </c>
+      <c r="E2">
+        <v>1.0</v>
+      </c>
+      <c r="F2">
+        <v>1.0</v>
+      </c>
+      <c r="G2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D3">
+        <v>1.6</v>
+      </c>
+      <c r="E3">
+        <v>1.6</v>
+      </c>
+      <c r="F3">
+        <v>1.6</v>
+      </c>
+      <c r="G3">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D4">
+        <v>3.41</v>
+      </c>
+      <c r="E4">
+        <v>3.41</v>
+      </c>
+      <c r="F4">
+        <v>3.41</v>
+      </c>
+      <c r="G4">
+        <v>3.41</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D5">
+        <v>12.33</v>
+      </c>
+      <c r="E5">
+        <v>12.33</v>
+      </c>
+      <c r="F5">
+        <v>12.33</v>
+      </c>
+      <c r="G5">
+        <v>12.33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D6">
+        <v>1.0</v>
+      </c>
+      <c r="E6">
+        <v>1.0</v>
+      </c>
+      <c r="F6">
+        <v>1.0</v>
+      </c>
+      <c r="G6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D7">
+        <v>1.92</v>
+      </c>
+      <c r="E7">
+        <v>1.92</v>
+      </c>
+      <c r="F7">
+        <v>1.92</v>
+      </c>
+      <c r="G7">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D8">
+        <v>4.66</v>
+      </c>
+      <c r="E8">
+        <v>4.66</v>
+      </c>
+      <c r="F8">
+        <v>4.66</v>
+      </c>
+      <c r="G8">
+        <v>4.66</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D9">
+        <v>9.68</v>
+      </c>
+      <c r="E9">
+        <v>9.68</v>
+      </c>
+      <c r="F9">
+        <v>9.68</v>
+      </c>
+      <c r="G9">
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D10">
+        <v>1.0</v>
+      </c>
+      <c r="E10">
+        <v>1.0</v>
+      </c>
+      <c r="F10">
+        <v>1.0</v>
+      </c>
+      <c r="G10">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D11">
+        <v>1.0</v>
+      </c>
+      <c r="E11">
+        <v>1.0</v>
+      </c>
+      <c r="F11">
+        <v>1.0</v>
+      </c>
+      <c r="G11">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D12">
+        <v>2.58</v>
+      </c>
+      <c r="E12">
+        <v>2.58</v>
+      </c>
+      <c r="F12">
+        <v>2.58</v>
+      </c>
+      <c r="G12">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D13">
+        <v>9.63</v>
+      </c>
+      <c r="E13">
+        <v>9.63</v>
+      </c>
+      <c r="F13">
+        <v>9.63</v>
+      </c>
+      <c r="G13">
+        <v>9.63</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D14">
+        <v>1.0</v>
+      </c>
+      <c r="E14">
+        <v>1.0</v>
+      </c>
+      <c r="F14">
+        <v>1.0</v>
+      </c>
+      <c r="G14">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D15">
+        <v>1.0</v>
+      </c>
+      <c r="E15">
+        <v>1.0</v>
+      </c>
+      <c r="F15">
+        <v>1.0</v>
+      </c>
+      <c r="G15">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D16">
+        <v>1.0</v>
+      </c>
+      <c r="E16">
+        <v>1.0</v>
+      </c>
+      <c r="F16">
+        <v>1.0</v>
+      </c>
+      <c r="G16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D17">
+        <v>1.0</v>
+      </c>
+      <c r="E17">
+        <v>1.0</v>
+      </c>
+      <c r="F17">
+        <v>1.0</v>
+      </c>
+      <c r="G17">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D18">
+        <v>1.0</v>
+      </c>
+      <c r="E18">
+        <v>1.0</v>
+      </c>
+      <c r="F18">
+        <v>1.0</v>
+      </c>
+      <c r="G18">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D19">
+        <v>1.65</v>
+      </c>
+      <c r="E19">
+        <v>1.65</v>
+      </c>
+      <c r="F19">
+        <v>1.65</v>
+      </c>
+      <c r="G19">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D20">
+        <v>2.73</v>
+      </c>
+      <c r="E20">
+        <v>2.73</v>
+      </c>
+      <c r="F20">
+        <v>2.73</v>
+      </c>
+      <c r="G20">
+        <v>2.73</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D21">
+        <v>11.21</v>
+      </c>
+      <c r="E21">
+        <v>11.21</v>
+      </c>
+      <c r="F21">
+        <v>11.21</v>
+      </c>
+      <c r="G21">
+        <v>11.21</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3794,7 +3866,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -4398,7 +4470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4414,16 +4486,16 @@
         <v>5</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
@@ -4687,7 +4759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4725,76 +4797,4 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="11">
-        <v>0.23981666666666668</v>
-      </c>
-      <c r="C2" s="11">
-        <v>0.23981666666666668</v>
-      </c>
-      <c r="D2" s="11">
-        <v>0.36586416666666666</v>
-      </c>
-      <c r="E2" s="11">
-        <v>0.29612333333333335</v>
-      </c>
-      <c r="F2" s="11">
-        <v>0.18924083333333333</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
combine breastfeeding promotion delivery options
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="74">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -213,6 +213,9 @@
     <t>Zinc supplementation</t>
   </si>
   <si>
+    <t>Complements group</t>
+  </si>
+  <si>
     <t>Complementary feeding (food secure with promotion)</t>
   </si>
   <si>
@@ -225,10 +228,7 @@
     <t>Complementary feeding (food insecure with neither promotion nor supplementation)</t>
   </si>
   <si>
-    <t>Breastfeeding promotion - Health system</t>
-  </si>
-  <si>
-    <t>Breastfeeding promotion - Home/community</t>
+    <t>Breastfeeding promotion - Health system &amp; Home/community</t>
   </si>
   <si>
     <t>pre-2016</t>
@@ -908,7 +908,9 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4"/>
+      <c r="A1" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -927,7 +929,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B2" s="4">
         <v>1.0</v>
@@ -947,7 +949,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4">
         <v>1.0</v>
@@ -967,7 +969,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="4">
         <v>1.0</v>
@@ -987,7 +989,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B5" s="4">
         <v>1.0</v>
@@ -1046,7 +1048,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B2" s="13">
         <v>2.3</v>
@@ -1065,24 +1067,12 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="13">
-        <v>2.3</v>
-      </c>
-      <c r="C3" s="13">
-        <v>4.6</v>
-      </c>
-      <c r="D3" s="13">
-        <v>1.57</v>
-      </c>
-      <c r="E3" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="14">
-        <v>1.0</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="4"/>
@@ -1091,14 +1081,6 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1164,10 +1146,10 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5" s="4">
-        <v>0.196</v>
+        <v>0.296</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -1176,10 +1158,10 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4">
-        <v>0.1</v>
+        <v>0.257</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -1187,11 +1169,11 @@
       <c r="G6" s="4"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>57</v>
+      <c r="A7" t="s">
+        <v>58</v>
       </c>
       <c r="B7" s="4">
-        <v>0.257</v>
+        <v>0.0</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -1199,24 +1181,19 @@
       <c r="G7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>58</v>
+      <c r="A8" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="B8" s="4">
         <v>0.0</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0.0</v>
-      </c>
+      <c r="B9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1266,10 +1243,7 @@
     </row>
     <row r="16">
       <c r="B16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="C16" s="4"/>
     </row>
     <row r="17">
       <c r="B17" s="4"/>
@@ -1314,10 +1288,6 @@
     <row r="27">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-    </row>
-    <row r="28">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
add unit cost and saturation coverage data
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="76">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -231,7 +231,13 @@
     <t>Breastfeeding promotion - Health system &amp; Home/community</t>
   </si>
   <si>
-    <t>pre-2016</t>
+    <t>baseline coverage</t>
+  </si>
+  <si>
+    <t>saturation coverage</t>
+  </si>
+  <si>
+    <t>unit cost</t>
   </si>
   <si>
     <t>Vitamin A supplementation</t>
@@ -336,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -378,6 +384,9 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1095,7 +1104,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="57.57"/>
-    <col customWidth="1" min="2" max="2" width="15.57"/>
+    <col customWidth="1" min="2" max="2" width="20.71"/>
+    <col customWidth="1" min="3" max="4" width="21.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1105,7 +1115,12 @@
       <c r="B1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
@@ -1114,32 +1129,46 @@
       <c r="B2" s="15">
         <v>0.0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="10"/>
+      <c r="C2" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="D2" s="4">
+        <v>60.0</v>
+      </c>
       <c r="E2" s="10"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B3" s="4">
         <v>0.19</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="C3" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="D3" s="4">
+        <v>300.0</v>
+      </c>
       <c r="E3" s="10"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B4" s="4">
         <v>0.385</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="C4" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="D4" s="4">
+        <v>300.0</v>
+      </c>
       <c r="E4" s="10"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1151,43 +1180,63 @@
       <c r="B5" s="4">
         <v>0.296</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="C5" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="D5" s="4">
+        <v>100.0</v>
+      </c>
       <c r="E5" s="10"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B6" s="4">
         <v>0.257</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="C6" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="D6" s="4">
+        <v>20.0</v>
+      </c>
       <c r="E6" s="10"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B7" s="4">
         <v>0.0</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="C7" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="D7" s="4">
+        <v>80.0</v>
+      </c>
       <c r="E7" s="10"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B8" s="4">
         <v>0.0</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="C8" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="D8" s="4">
+        <v>90.0</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1309,7 +1358,7 @@
         <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
         <v>36</v>
@@ -1326,10 +1375,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C2" s="16">
         <v>0.35</v>
@@ -1346,27 +1395,27 @@
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="16">
-        <v>0.0</v>
+        <v>64</v>
+      </c>
+      <c r="C3" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0.1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C4" s="16">
         <v>0.31</v>
@@ -1383,7 +1432,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C5" s="16">
         <v>0.336</v>
@@ -1400,10 +1449,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C6" s="16">
         <v>0.09</v>
@@ -1420,7 +1469,7 @@
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C7" s="16">
         <v>1.0</v>
@@ -1452,7 +1501,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -1489,10 +1538,10 @@
       <c r="E2" s="4">
         <v>0.0</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="18">
         <v>0.253</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="18">
         <v>0.253</v>
       </c>
     </row>
@@ -1510,16 +1559,16 @@
       <c r="E3" s="4">
         <v>0.0</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="18">
         <v>0.253</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="18">
         <v>0.253</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -1533,10 +1582,10 @@
       <c r="E4" s="4">
         <v>0.416</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="19">
         <v>0.416</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="19">
         <v>0.416</v>
       </c>
     </row>
@@ -1970,7 +2019,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -2037,7 +2086,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -2113,7 +2162,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -2180,7 +2229,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -2256,19 +2305,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2">
@@ -2276,7 +2325,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C2" s="4">
         <v>3.14</v>
@@ -2291,7 +2340,7 @@
     <row r="3">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C3" s="4">
         <v>1.6</v>
@@ -2306,7 +2355,7 @@
     <row r="4">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C4" s="4">
         <v>1.6</v>
@@ -2323,7 +2372,7 @@
         <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C5" s="4">
         <v>1.75</v>
@@ -2337,7 +2386,7 @@
     </row>
     <row r="6">
       <c r="B6" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C6" s="4">
         <v>1.4</v>
@@ -2351,7 +2400,7 @@
     </row>
     <row r="7">
       <c r="B7" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C7" s="4">
         <v>1.4</v>
@@ -2368,7 +2417,7 @@
         <v>38</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C8" s="4">
         <v>1.52</v>
@@ -2382,7 +2431,7 @@
     </row>
     <row r="9">
       <c r="B9" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C9" s="4">
         <v>1.2</v>
@@ -2396,7 +2445,7 @@
     </row>
     <row r="10">
       <c r="B10" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C10" s="4">
         <v>1.2</v>
@@ -2422,22 +2471,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B2" s="4">
         <v>0.0543</v>
@@ -2451,7 +2500,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B3" s="4">
         <v>0.009</v>
@@ -2465,7 +2514,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B4" s="4">
         <v>0.0</v>
@@ -2491,16 +2540,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2">
@@ -2531,19 +2580,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
replace exclusive with age-appropriate breastfeeding promotion
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -18,16 +18,18 @@
     <sheet state="visible" name="OR stunting by birth outcome" sheetId="13" r:id="rId15"/>
     <sheet state="visible" name="OR stunting by intervention" sheetId="14" r:id="rId16"/>
     <sheet state="visible" name="OR stunting for complements" sheetId="15" r:id="rId17"/>
-    <sheet state="visible" name="OR exclusiveBF by intervention" sheetId="16" r:id="rId18"/>
-    <sheet state="visible" name="Interventions coverages" sheetId="17" r:id="rId19"/>
-    <sheet state="visible" name="Interventions maternal" sheetId="18" r:id="rId20"/>
-    <sheet state="visible" name="Interventions affected fraction" sheetId="19" r:id="rId21"/>
-    <sheet state="visible" name="Interventions mortality eff" sheetId="20" r:id="rId22"/>
-    <sheet state="visible" name="Interventions incidence eff" sheetId="21" r:id="rId23"/>
-    <sheet state="visible" name="RR birth by type" sheetId="22" r:id="rId24"/>
-    <sheet state="visible" name="birth distribution" sheetId="23" r:id="rId25"/>
-    <sheet state="visible" name="time between births" sheetId="24" r:id="rId26"/>
-    <sheet state="visible" name="RR birth by time" sheetId="25" r:id="rId27"/>
+    <sheet state="visible" name="OR appropriateBF by interv" sheetId="16" r:id="rId18"/>
+    <sheet state="visible" name="Appropriate breastfeeding" sheetId="17" r:id="rId19"/>
+    <sheet state="visible" name="Interventions coverages" sheetId="18" r:id="rId20"/>
+    <sheet state="visible" name="Interventions target population" sheetId="19" r:id="rId21"/>
+    <sheet state="visible" name="Interventions maternal" sheetId="20" r:id="rId22"/>
+    <sheet state="visible" name="Interventions affected fraction" sheetId="21" r:id="rId23"/>
+    <sheet state="visible" name="Interventions mortality eff" sheetId="22" r:id="rId24"/>
+    <sheet state="visible" name="Interventions incidence eff" sheetId="23" r:id="rId25"/>
+    <sheet state="visible" name="RR birth by type" sheetId="24" r:id="rId26"/>
+    <sheet state="visible" name="birth distribution" sheetId="25" r:id="rId27"/>
+    <sheet state="visible" name="time between births" sheetId="26" r:id="rId28"/>
+    <sheet state="visible" name="RR birth by time" sheetId="27" r:id="rId29"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -67,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="77">
   <si>
     <t>&lt;1 month</t>
   </si>
@@ -253,6 +255,9 @@
   </si>
   <si>
     <t>Multiple micronutrient supplementation</t>
+  </si>
+  <si>
+    <t>pregnant women</t>
   </si>
   <si>
     <t>Outcome</t>
@@ -342,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -380,6 +385,9 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
@@ -473,6 +481,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing26.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/worksheetdrawing27.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
@@ -1028,11 +1044,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="37.29"/>
-    <col customWidth="1" min="2" max="2" width="10.71"/>
-    <col customWidth="1" min="3" max="3" width="12.71"/>
-    <col customWidth="1" min="4" max="4" width="11.14"/>
-    <col customWidth="1" min="5" max="6" width="12.29"/>
+    <col customWidth="1" min="1" max="1" width="43.14"/>
+    <col customWidth="1" min="2" max="6" width="13.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1097,6 +1110,69 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="5" width="13.43"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1126,7 +1202,7 @@
       <c r="A2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="16">
         <v>0.0</v>
       </c>
       <c r="C2" s="4">
@@ -1343,7 +1419,593 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="57.57"/>
+    <col customWidth="1" min="2" max="6" width="13.57"/>
+    <col customWidth="1" min="7" max="7" width="17.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13">
+      <c r="B13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.003996</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.15484515</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.06893107</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.30969031</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.25974026</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.00899101</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.13186813</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.06193806</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.131</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.131</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.131</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.131</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.203</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.203</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.203</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.203</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.006</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.006</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.006</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.006</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.09300000000000001</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.09300000000000001</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.09300000000000001</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.09300000000000001</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.034</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.034</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.034</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.102</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.102</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.102</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.102</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.11599999999999999</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.11599999999999999</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.11599999999999999</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.11599999999999999</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.285</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.285</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.285</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.285</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1358,7 +2020,7 @@
         <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
         <v>36</v>
@@ -1378,35 +2040,35 @@
         <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="16">
+        <v>64</v>
+      </c>
+      <c r="C2" s="17">
         <v>0.35</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="17">
         <v>0.35</v>
       </c>
-      <c r="E2" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="16">
+      <c r="E2" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="17">
         <v>0.0</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="17">
+        <v>65</v>
+      </c>
+      <c r="C3" s="18">
         <v>0.1</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="18">
         <v>0.1</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="18">
         <v>0.1</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="18">
         <v>0.1</v>
       </c>
     </row>
@@ -1415,35 +2077,35 @@
         <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="16">
+        <v>64</v>
+      </c>
+      <c r="C4" s="17">
         <v>0.31</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="17">
         <v>0.31</v>
       </c>
-      <c r="E4" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="16">
+      <c r="E4" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="17">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="16">
+        <v>65</v>
+      </c>
+      <c r="C5" s="17">
         <v>0.336</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="17">
         <v>0.336</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="17">
         <v>0.336</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="17">
         <v>0.0</v>
       </c>
     </row>
@@ -1452,35 +2114,35 @@
         <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="16">
+        <v>64</v>
+      </c>
+      <c r="C6" s="17">
         <v>0.09</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="17">
         <v>0.09</v>
       </c>
-      <c r="E6" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="16">
+      <c r="E6" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="17">
         <v>0.0</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="16">
+        <v>65</v>
+      </c>
+      <c r="C7" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="17">
         <v>0.0</v>
       </c>
     </row>
@@ -1489,7 +2151,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1501,7 +2163,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -1538,10 +2200,10 @@
       <c r="E2" s="4">
         <v>0.0</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="19">
         <v>0.253</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="19">
         <v>0.253</v>
       </c>
     </row>
@@ -1559,10 +2221,10 @@
       <c r="E3" s="4">
         <v>0.0</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="19">
         <v>0.253</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="19">
         <v>0.253</v>
       </c>
     </row>
@@ -1582,10 +2244,10 @@
       <c r="E4" s="4">
         <v>0.416</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="20">
         <v>0.416</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="20">
         <v>0.416</v>
       </c>
     </row>
@@ -1635,379 +2297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.003996</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.15484515</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.06893107</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0.30969031</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.25974026</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.00899101</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.13186813</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.06193806</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.131</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.131</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.131</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.131</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.203</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.203</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.203</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.203</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0.03</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0.03</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0.03</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.006</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.006</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.006</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0.006</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.09300000000000001</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.09300000000000001</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.09300000000000001</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.09300000000000001</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0.034</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.034</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.034</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.034</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0.102</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.102</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0.102</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0.102</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0.11599999999999999</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.11599999999999999</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0.11599999999999999</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0.11599999999999999</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0.285</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.285</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0.285</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.285</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2019,7 +2309,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -2147,315 +2437,6 @@
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.52</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="4">
-        <v>3.14</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1.73</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1.75</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1.75</v>
-      </c>
-      <c r="E5" s="4">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1.52</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1.52</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1.0</v>
-      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2474,57 +2455,131 @@
         <v>66</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.0543</v>
+        <v>47</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C2" s="4">
-        <v>0.1711</v>
+        <v>0.0</v>
       </c>
       <c r="D2" s="4">
-        <v>3.0E-4</v>
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.65</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.009</v>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C3" s="4">
-        <v>0.3607</v>
+        <v>0.0</v>
       </c>
       <c r="D3" s="4">
-        <v>0.0085</v>
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.52</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0.0</v>
+        <v>57</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="4">
-        <v>0.2908</v>
+        <v>0.0</v>
       </c>
       <c r="D4" s="4">
-        <v>0.1048</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2540,30 +2595,156 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="4" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3.14</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.73</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4">
-        <v>0.2258</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.0705</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.134</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.5698</v>
+      <c r="C4" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1.52</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.52</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -2580,19 +2761,128 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.0543</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.1711</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3.0E-4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.009</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.3607</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.0085</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.2908</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.1048</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="C1" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4">
+        <v>0.2258</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.0705</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.134</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.5698</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="E1" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
shorten name of breastfeeding promotion
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -230,7 +230,7 @@
     <t>Complementary feeding (food insecure with neither promotion nor supplementation)</t>
   </si>
   <si>
-    <t>Breastfeeding promotion - Health system &amp; Home/community</t>
+    <t>Breastfeeding promotion (dual delivery)</t>
   </si>
   <si>
     <t>baseline coverage</t>
@@ -1179,7 +1179,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="57.57"/>
+    <col customWidth="1" min="1" max="1" width="37.86"/>
     <col customWidth="1" min="2" max="2" width="20.71"/>
     <col customWidth="1" min="3" max="4" width="21.43"/>
   </cols>
@@ -1426,7 +1426,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="57.57"/>
+    <col customWidth="1" min="1" max="1" width="37.71"/>
     <col customWidth="1" min="2" max="6" width="13.57"/>
     <col customWidth="1" min="7" max="7" width="17.29"/>
   </cols>

</xml_diff>

<commit_message>
complete target populations matrix and add to both spreadsheets
</commit_message>
<xml_diff>
--- a/InputForCode.xlsx
+++ b/InputForCode.xlsx
@@ -347,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -391,6 +391,9 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
@@ -1458,78 +1461,162 @@
       <c r="A2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="B2" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="F2" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="G2" s="17">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="B3" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="C3" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="G3" s="17">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="B4" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="F4" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="17">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="B5" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="B6" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="C6" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="G6" s="17">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="B7" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="F7" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="G7" s="17">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="B8" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="C8" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="17">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="4"/>
@@ -2042,16 +2129,16 @@
       <c r="B2" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="18">
         <v>0.35</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="18">
         <v>0.35</v>
       </c>
-      <c r="E2" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="17">
+      <c r="E2" s="18">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="18">
         <v>0.0</v>
       </c>
     </row>
@@ -2059,16 +2146,16 @@
       <c r="B3" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="19">
         <v>0.1</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="19">
         <v>0.1</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="19">
         <v>0.1</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="19">
         <v>0.1</v>
       </c>
     </row>
@@ -2079,16 +2166,16 @@
       <c r="B4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="18">
         <v>0.31</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="18">
         <v>0.31</v>
       </c>
-      <c r="E4" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="17">
+      <c r="E4" s="18">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="18">
         <v>0.0</v>
       </c>
     </row>
@@ -2096,16 +2183,16 @@
       <c r="B5" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="18">
         <v>0.336</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="18">
         <v>0.336</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="18">
         <v>0.336</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="18">
         <v>0.0</v>
       </c>
     </row>
@@ -2116,16 +2203,16 @@
       <c r="B6" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="18">
         <v>0.09</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="18">
         <v>0.09</v>
       </c>
-      <c r="E6" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="17">
+      <c r="E6" s="18">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="18">
         <v>0.0</v>
       </c>
     </row>
@@ -2133,16 +2220,16 @@
       <c r="B7" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="17">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="17">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="17">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="17">
+      <c r="C7" s="18">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="18">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="18">
         <v>0.0</v>
       </c>
     </row>
@@ -2200,10 +2287,10 @@
       <c r="E2" s="4">
         <v>0.0</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="20">
         <v>0.253</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="20">
         <v>0.253</v>
       </c>
     </row>
@@ -2221,10 +2308,10 @@
       <c r="E3" s="4">
         <v>0.0</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="20">
         <v>0.253</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="20">
         <v>0.253</v>
       </c>
     </row>
@@ -2244,10 +2331,10 @@
       <c r="E4" s="4">
         <v>0.416</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="21">
         <v>0.416</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="21">
         <v>0.416</v>
       </c>
     </row>

</xml_diff>